<commit_message>
warnings added and grant type validation updated
</commit_message>
<xml_diff>
--- a/core/test/input/FullValuesOnly.xlsx
+++ b/core/test/input/FullValuesOnly.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="245" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="245" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="DOC_SRC" sheetId="1" state="visible" r:id="rId2"/>
@@ -1168,17 +1168,17 @@
   </sheetPr>
   <dimension ref="A1:T68"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100">
-      <selection activeCell="A6" activeCellId="0" pane="topLeft" sqref="A6"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A40" view="normal" windowProtection="false" workbookViewId="0" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100">
+      <selection activeCell="C56" activeCellId="0" pane="topLeft" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.643137254902"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.8901960784314"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.0235294117647"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.2"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.5176470588235"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.7529411764706"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.6549019607843"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.9019607843137"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.043137254902"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.2196078431373"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.5333333333333"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.7607843137255"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="1">
@@ -1449,7 +1449,7 @@
         <v>10</v>
       </c>
       <c r="C26" s="4" t="n">
-        <v>38353</v>
+        <v>41060</v>
       </c>
       <c r="D26" s="19"/>
       <c r="E26" s="20"/>
@@ -1600,7 +1600,7 @@
         <v>10</v>
       </c>
       <c r="C41" s="4" t="n">
-        <v>40909</v>
+        <v>40544</v>
       </c>
       <c r="D41" s="22"/>
       <c r="E41" s="23"/>
@@ -1749,7 +1749,7 @@
         <v>10</v>
       </c>
       <c r="C56" s="4" t="n">
-        <v>41275</v>
+        <v>40179</v>
       </c>
       <c r="D56" s="22"/>
       <c r="E56" s="23"/>
@@ -1900,7 +1900,7 @@
   </sheetPr>
   <dimension ref="A1:BF8"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="T1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="T1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
       <selection activeCell="AC29" activeCellId="0" pane="topLeft" sqref="AC29"/>
     </sheetView>
   </sheetViews>
@@ -2649,140 +2649,140 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.0862745098039"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.2627450980392"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.92156862745098"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.0039215686275"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.9137254901961"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.4666666666667"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.3921568627451"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.4470588235294"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.6509803921569"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="18.6823529411765"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="15.3098039215686"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.6039215686275"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="11.9411764705882"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="13.7921568627451"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="12.9450980392157"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.956862745098"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="16.4823529411765"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.2705882352941"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="16.3176470588235"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="13.956862745098"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="10.2627450980392"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="10.7607843137255"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="8.08235294117647"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.1058823529412"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.2705882352941"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.92941176470588"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.0196078431373"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.9333333333333"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.478431372549"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.4039215686274"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.4549019607843"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.6627450980392"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="18.6941176470588"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="15.321568627451"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.6117647058824"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="11.9490196078431"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="13.8"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="12.9529411764706"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.9647058823529"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="16.4941176470588"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.278431372549"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="16.3254901960784"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="13.9647058823529"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="10.2705882352941"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="10.7686274509804"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="8.09019607843137"/>
     <col collapsed="false" hidden="false" max="24" min="24" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="11.6078431372549"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="11.6196078431373"/>
     <col collapsed="false" hidden="false" max="26" min="26" style="0" width="5.52549019607843"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="11.6078431372549"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="14.1254901960784"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="10.7607843137255"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="8.08235294117647"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="11.6196078431373"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="14.1333333333333"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="10.7686274509804"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="8.09019607843137"/>
     <col collapsed="false" hidden="false" max="31" min="31" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="11.6078431372549"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="11.6196078431373"/>
     <col collapsed="false" hidden="false" max="33" min="33" style="0" width="5.52549019607843"/>
     <col collapsed="false" hidden="false" max="34" min="34" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="14.6392156862745"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="10.7607843137255"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="8.08235294117647"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="14.6509803921569"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="10.7686274509804"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="8.09019607843137"/>
     <col collapsed="false" hidden="false" max="38" min="38" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="11.6078431372549"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="11.6196078431373"/>
     <col collapsed="false" hidden="false" max="40" min="40" style="0" width="5.52549019607843"/>
     <col collapsed="false" hidden="false" max="41" min="41" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="14.2980392156863"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="10.7607843137255"/>
-    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="8.08235294117647"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="14.3058823529412"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="10.7686274509804"/>
+    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="8.09019607843137"/>
     <col collapsed="false" hidden="false" max="45" min="45" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="11.6078431372549"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="11.6196078431373"/>
     <col collapsed="false" hidden="false" max="47" min="47" style="0" width="5.52549019607843"/>
     <col collapsed="false" hidden="false" max="48" min="48" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="49" min="49" style="0" width="14.7960784313726"/>
-    <col collapsed="false" hidden="false" max="50" min="50" style="0" width="10.7607843137255"/>
-    <col collapsed="false" hidden="false" max="51" min="51" style="0" width="8.08235294117647"/>
+    <col collapsed="false" hidden="false" max="49" min="49" style="0" width="14.8039215686275"/>
+    <col collapsed="false" hidden="false" max="50" min="50" style="0" width="10.7686274509804"/>
+    <col collapsed="false" hidden="false" max="51" min="51" style="0" width="8.09019607843137"/>
     <col collapsed="false" hidden="false" max="52" min="52" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="53" min="53" style="0" width="11.6078431372549"/>
+    <col collapsed="false" hidden="false" max="53" min="53" style="0" width="11.6196078431373"/>
     <col collapsed="false" hidden="false" max="54" min="54" style="0" width="5.52549019607843"/>
     <col collapsed="false" hidden="false" max="55" min="55" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="56" min="56" style="0" width="15.1372549019608"/>
-    <col collapsed="false" hidden="false" max="57" min="57" style="0" width="10.7607843137255"/>
-    <col collapsed="false" hidden="false" max="58" min="58" style="0" width="8.08235294117647"/>
+    <col collapsed="false" hidden="false" max="56" min="56" style="0" width="15.1490196078431"/>
+    <col collapsed="false" hidden="false" max="57" min="57" style="0" width="10.7686274509804"/>
+    <col collapsed="false" hidden="false" max="58" min="58" style="0" width="8.09019607843137"/>
     <col collapsed="false" hidden="false" max="59" min="59" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="60" min="60" style="0" width="11.6078431372549"/>
+    <col collapsed="false" hidden="false" max="60" min="60" style="0" width="11.6196078431373"/>
     <col collapsed="false" hidden="false" max="61" min="61" style="0" width="5.52549019607843"/>
     <col collapsed="false" hidden="false" max="62" min="62" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="63" min="63" style="0" width="10.2627450980392"/>
-    <col collapsed="false" hidden="false" max="64" min="64" style="0" width="8.08235294117647"/>
+    <col collapsed="false" hidden="false" max="63" min="63" style="0" width="10.2705882352941"/>
+    <col collapsed="false" hidden="false" max="64" min="64" style="0" width="8.09019607843137"/>
     <col collapsed="false" hidden="false" max="65" min="65" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="66" min="66" style="0" width="11.6078431372549"/>
+    <col collapsed="false" hidden="false" max="66" min="66" style="0" width="11.6196078431373"/>
     <col collapsed="false" hidden="false" max="67" min="67" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="68" min="68" style="0" width="13.956862745098"/>
-    <col collapsed="false" hidden="false" max="69" min="69" style="0" width="8.08235294117647"/>
+    <col collapsed="false" hidden="false" max="68" min="68" style="0" width="13.9647058823529"/>
+    <col collapsed="false" hidden="false" max="69" min="69" style="0" width="8.09019607843137"/>
     <col collapsed="false" hidden="false" max="70" min="70" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="71" min="71" style="0" width="11.6078431372549"/>
+    <col collapsed="false" hidden="false" max="71" min="71" style="0" width="11.6196078431373"/>
     <col collapsed="false" hidden="false" max="72" min="72" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="73" min="73" style="0" width="12.9450980392157"/>
-    <col collapsed="false" hidden="false" max="74" min="74" style="0" width="8.08235294117647"/>
+    <col collapsed="false" hidden="false" max="73" min="73" style="0" width="12.9529411764706"/>
+    <col collapsed="false" hidden="false" max="74" min="74" style="0" width="8.09019607843137"/>
     <col collapsed="false" hidden="false" max="75" min="75" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="76" min="76" style="0" width="11.6078431372549"/>
+    <col collapsed="false" hidden="false" max="76" min="76" style="0" width="11.6196078431373"/>
     <col collapsed="false" hidden="false" max="77" min="77" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="78" min="78" style="0" width="12.7764705882353"/>
-    <col collapsed="false" hidden="false" max="79" min="79" style="0" width="8.08235294117647"/>
+    <col collapsed="false" hidden="false" max="78" min="78" style="0" width="12.7882352941176"/>
+    <col collapsed="false" hidden="false" max="79" min="79" style="0" width="8.09019607843137"/>
     <col collapsed="false" hidden="false" max="80" min="80" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="81" min="81" style="0" width="11.6078431372549"/>
+    <col collapsed="false" hidden="false" max="81" min="81" style="0" width="11.6196078431373"/>
     <col collapsed="false" hidden="false" max="82" min="82" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="83" min="83" style="0" width="13.6352941176471"/>
-    <col collapsed="false" hidden="false" max="84" min="84" style="0" width="8.08235294117647"/>
+    <col collapsed="false" hidden="false" max="83" min="83" style="0" width="13.643137254902"/>
+    <col collapsed="false" hidden="false" max="84" min="84" style="0" width="8.09019607843137"/>
     <col collapsed="false" hidden="false" max="85" min="85" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="86" min="86" style="0" width="11.6078431372549"/>
+    <col collapsed="false" hidden="false" max="86" min="86" style="0" width="11.6196078431373"/>
     <col collapsed="false" hidden="false" max="87" min="87" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="88" min="88" style="0" width="14.7960784313726"/>
-    <col collapsed="false" hidden="false" max="89" min="89" style="0" width="8.08235294117647"/>
+    <col collapsed="false" hidden="false" max="88" min="88" style="0" width="14.8039215686275"/>
+    <col collapsed="false" hidden="false" max="89" min="89" style="0" width="8.09019607843137"/>
     <col collapsed="false" hidden="false" max="90" min="90" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="91" min="91" style="0" width="11.6078431372549"/>
+    <col collapsed="false" hidden="false" max="91" min="91" style="0" width="11.6196078431373"/>
     <col collapsed="false" hidden="false" max="92" min="92" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="93" min="93" style="0" width="10.2627450980392"/>
-    <col collapsed="false" hidden="false" max="94" min="94" style="0" width="13.7921568627451"/>
-    <col collapsed="false" hidden="false" max="95" min="95" style="0" width="14.7960784313726"/>
-    <col collapsed="false" hidden="false" max="96" min="96" style="0" width="17.321568627451"/>
+    <col collapsed="false" hidden="false" max="93" min="93" style="0" width="10.2705882352941"/>
+    <col collapsed="false" hidden="false" max="94" min="94" style="0" width="13.8"/>
+    <col collapsed="false" hidden="false" max="95" min="95" style="0" width="14.8039215686275"/>
+    <col collapsed="false" hidden="false" max="96" min="96" style="0" width="17.3372549019608"/>
     <col collapsed="false" hidden="false" max="97" min="97" style="0" width="6.02352941176471"/>
-    <col collapsed="false" hidden="false" max="98" min="98" style="0" width="23.0313725490196"/>
-    <col collapsed="false" hidden="false" max="99" min="99" style="0" width="15.9764705882353"/>
-    <col collapsed="false" hidden="false" max="100" min="100" style="0" width="17.1529411764706"/>
-    <col collapsed="false" hidden="false" max="101" min="101" style="0" width="17.321568627451"/>
+    <col collapsed="false" hidden="false" max="98" min="98" style="0" width="23.043137254902"/>
+    <col collapsed="false" hidden="false" max="99" min="99" style="0" width="15.9921568627451"/>
+    <col collapsed="false" hidden="false" max="100" min="100" style="0" width="17.1647058823529"/>
+    <col collapsed="false" hidden="false" max="101" min="101" style="0" width="17.3372549019608"/>
     <col collapsed="false" hidden="false" max="102" min="102" style="0" width="6.02352941176471"/>
-    <col collapsed="false" hidden="false" max="103" min="103" style="0" width="22.1960784313725"/>
-    <col collapsed="false" hidden="false" max="104" min="104" style="0" width="15.9764705882353"/>
-    <col collapsed="false" hidden="false" max="105" min="105" style="0" width="17.1529411764706"/>
-    <col collapsed="false" hidden="false" max="106" min="106" style="0" width="17.321568627451"/>
+    <col collapsed="false" hidden="false" max="103" min="103" style="0" width="22.2117647058824"/>
+    <col collapsed="false" hidden="false" max="104" min="104" style="0" width="15.9921568627451"/>
+    <col collapsed="false" hidden="false" max="105" min="105" style="0" width="17.1647058823529"/>
+    <col collapsed="false" hidden="false" max="106" min="106" style="0" width="17.3372549019608"/>
     <col collapsed="false" hidden="false" max="107" min="107" style="0" width="6.02352941176471"/>
-    <col collapsed="false" hidden="false" max="108" min="108" style="0" width="11.7725490196078"/>
-    <col collapsed="false" hidden="false" max="109" min="109" style="0" width="17.321568627451"/>
-    <col collapsed="false" hidden="false" max="110" min="110" style="0" width="12.7764705882353"/>
-    <col collapsed="false" hidden="false" max="111" min="111" style="0" width="18.5098039215686"/>
-    <col collapsed="false" hidden="false" max="112" min="112" style="0" width="17.321568627451"/>
-    <col collapsed="false" hidden="false" max="113" min="113" style="0" width="12.7764705882353"/>
-    <col collapsed="false" hidden="false" max="114" min="114" style="0" width="19.5137254901961"/>
-    <col collapsed="false" hidden="false" max="115" min="115" style="0" width="17.321568627451"/>
-    <col collapsed="false" hidden="false" max="116" min="116" style="0" width="12.7764705882353"/>
-    <col collapsed="false" hidden="false" max="117" min="117" style="0" width="18.6823529411765"/>
-    <col collapsed="false" hidden="false" max="119" min="118" style="0" width="17.321568627451"/>
-    <col collapsed="false" hidden="false" max="120" min="120" style="0" width="16.4823529411765"/>
-    <col collapsed="false" hidden="false" max="121" min="121" style="0" width="11.7725490196078"/>
-    <col collapsed="false" hidden="false" max="122" min="122" style="0" width="15.6509803921569"/>
-    <col collapsed="false" hidden="false" max="123" min="123" style="0" width="16.3176470588235"/>
-    <col collapsed="false" hidden="false" max="124" min="124" style="0" width="18.5098039215686"/>
-    <col collapsed="false" hidden="false" max="125" min="125" style="0" width="14.4627450980392"/>
-    <col collapsed="false" hidden="false" max="126" min="126" style="0" width="13.6352941176471"/>
-    <col collapsed="false" hidden="false" max="138" min="127" style="0" width="18.6823529411765"/>
-    <col collapsed="false" hidden="false" max="140" min="139" style="0" width="30.9490196078431"/>
-    <col collapsed="false" hidden="false" max="141" min="141" style="0" width="26.0823529411765"/>
-    <col collapsed="false" hidden="false" max="142" min="142" style="0" width="20.6941176470588"/>
-    <col collapsed="false" hidden="false" max="143" min="143" style="0" width="13.1098039215686"/>
+    <col collapsed="false" hidden="false" max="108" min="108" style="0" width="11.7764705882353"/>
+    <col collapsed="false" hidden="false" max="109" min="109" style="0" width="17.3372549019608"/>
+    <col collapsed="false" hidden="false" max="110" min="110" style="0" width="12.7882352941176"/>
+    <col collapsed="false" hidden="false" max="111" min="111" style="0" width="18.521568627451"/>
+    <col collapsed="false" hidden="false" max="112" min="112" style="0" width="17.3372549019608"/>
+    <col collapsed="false" hidden="false" max="113" min="113" style="0" width="12.7882352941176"/>
+    <col collapsed="false" hidden="false" max="114" min="114" style="0" width="19.5254901960784"/>
+    <col collapsed="false" hidden="false" max="115" min="115" style="0" width="17.3372549019608"/>
+    <col collapsed="false" hidden="false" max="116" min="116" style="0" width="12.7882352941176"/>
+    <col collapsed="false" hidden="false" max="117" min="117" style="0" width="18.6941176470588"/>
+    <col collapsed="false" hidden="false" max="119" min="118" style="0" width="17.3372549019608"/>
+    <col collapsed="false" hidden="false" max="120" min="120" style="0" width="16.4941176470588"/>
+    <col collapsed="false" hidden="false" max="121" min="121" style="0" width="11.7764705882353"/>
+    <col collapsed="false" hidden="false" max="122" min="122" style="0" width="15.6627450980392"/>
+    <col collapsed="false" hidden="false" max="123" min="123" style="0" width="16.3254901960784"/>
+    <col collapsed="false" hidden="false" max="124" min="124" style="0" width="18.521568627451"/>
+    <col collapsed="false" hidden="false" max="125" min="125" style="0" width="14.4666666666667"/>
+    <col collapsed="false" hidden="false" max="126" min="126" style="0" width="13.643137254902"/>
+    <col collapsed="false" hidden="false" max="138" min="127" style="0" width="18.6941176470588"/>
+    <col collapsed="false" hidden="false" max="140" min="139" style="0" width="30.9725490196078"/>
+    <col collapsed="false" hidden="false" max="141" min="141" style="0" width="26.1019607843137"/>
+    <col collapsed="false" hidden="false" max="142" min="142" style="0" width="20.7098039215686"/>
+    <col collapsed="false" hidden="false" max="143" min="143" style="0" width="13.121568627451"/>
     <col collapsed="false" hidden="false" max="144" min="144" style="0" width="7.74117647058824"/>
-    <col collapsed="false" hidden="false" max="145" min="145" style="0" width="13.4509803921569"/>
-    <col collapsed="false" hidden="false" max="146" min="146" style="0" width="10.4274509803922"/>
-    <col collapsed="false" hidden="false" max="1025" min="147" style="0" width="18.6823529411765"/>
+    <col collapsed="false" hidden="false" max="145" min="145" style="0" width="13.4588235294118"/>
+    <col collapsed="false" hidden="false" max="146" min="146" style="0" width="10.4313725490196"/>
+    <col collapsed="false" hidden="false" max="1025" min="147" style="0" width="18.6941176470588"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="1">
@@ -7519,140 +7519,140 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.0862745098039"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.2627450980392"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.92156862745098"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.0039215686275"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.9137254901961"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.4666666666667"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.3921568627451"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.4470588235294"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.6509803921569"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="18.6823529411765"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="15.3098039215686"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.6039215686275"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="11.9411764705882"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="13.7921568627451"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="12.9450980392157"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.956862745098"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="16.4823529411765"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.2705882352941"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="16.3176470588235"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="13.956862745098"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="10.2627450980392"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="10.7607843137255"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="8.08235294117647"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.1058823529412"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.2705882352941"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.92941176470588"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.0196078431373"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.9333333333333"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.478431372549"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.4039215686274"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.4549019607843"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.6627450980392"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="18.6941176470588"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="15.321568627451"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.6117647058824"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="11.9490196078431"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="13.8"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="12.9529411764706"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.9647058823529"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="16.4941176470588"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.278431372549"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="16.3254901960784"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="13.9647058823529"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="10.2705882352941"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="10.7686274509804"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="8.09019607843137"/>
     <col collapsed="false" hidden="false" max="24" min="24" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="11.6078431372549"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="11.6196078431373"/>
     <col collapsed="false" hidden="false" max="26" min="26" style="0" width="5.52549019607843"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="11.6078431372549"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="14.1254901960784"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="10.7607843137255"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="8.08235294117647"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="11.6196078431373"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="14.1333333333333"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="10.7686274509804"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="8.09019607843137"/>
     <col collapsed="false" hidden="false" max="31" min="31" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="11.6078431372549"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="11.6196078431373"/>
     <col collapsed="false" hidden="false" max="33" min="33" style="0" width="5.52549019607843"/>
     <col collapsed="false" hidden="false" max="34" min="34" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="14.6392156862745"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="10.7607843137255"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="8.08235294117647"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="14.6509803921569"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="10.7686274509804"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="8.09019607843137"/>
     <col collapsed="false" hidden="false" max="38" min="38" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="11.6078431372549"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="11.6196078431373"/>
     <col collapsed="false" hidden="false" max="40" min="40" style="0" width="5.52549019607843"/>
     <col collapsed="false" hidden="false" max="41" min="41" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="14.2980392156863"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="10.7607843137255"/>
-    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="8.08235294117647"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="14.3058823529412"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="10.7686274509804"/>
+    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="8.09019607843137"/>
     <col collapsed="false" hidden="false" max="45" min="45" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="11.6078431372549"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="11.6196078431373"/>
     <col collapsed="false" hidden="false" max="47" min="47" style="0" width="5.52549019607843"/>
     <col collapsed="false" hidden="false" max="48" min="48" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="49" min="49" style="0" width="14.7960784313726"/>
-    <col collapsed="false" hidden="false" max="50" min="50" style="0" width="10.7607843137255"/>
-    <col collapsed="false" hidden="false" max="51" min="51" style="0" width="8.08235294117647"/>
+    <col collapsed="false" hidden="false" max="49" min="49" style="0" width="14.8039215686275"/>
+    <col collapsed="false" hidden="false" max="50" min="50" style="0" width="10.7686274509804"/>
+    <col collapsed="false" hidden="false" max="51" min="51" style="0" width="8.09019607843137"/>
     <col collapsed="false" hidden="false" max="52" min="52" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="53" min="53" style="0" width="11.6078431372549"/>
+    <col collapsed="false" hidden="false" max="53" min="53" style="0" width="11.6196078431373"/>
     <col collapsed="false" hidden="false" max="54" min="54" style="0" width="5.52549019607843"/>
     <col collapsed="false" hidden="false" max="55" min="55" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="56" min="56" style="0" width="15.1372549019608"/>
-    <col collapsed="false" hidden="false" max="57" min="57" style="0" width="10.7607843137255"/>
-    <col collapsed="false" hidden="false" max="58" min="58" style="0" width="8.08235294117647"/>
+    <col collapsed="false" hidden="false" max="56" min="56" style="0" width="15.1490196078431"/>
+    <col collapsed="false" hidden="false" max="57" min="57" style="0" width="10.7686274509804"/>
+    <col collapsed="false" hidden="false" max="58" min="58" style="0" width="8.09019607843137"/>
     <col collapsed="false" hidden="false" max="59" min="59" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="60" min="60" style="0" width="11.6078431372549"/>
+    <col collapsed="false" hidden="false" max="60" min="60" style="0" width="11.6196078431373"/>
     <col collapsed="false" hidden="false" max="61" min="61" style="0" width="5.52549019607843"/>
     <col collapsed="false" hidden="false" max="62" min="62" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="63" min="63" style="0" width="10.2627450980392"/>
-    <col collapsed="false" hidden="false" max="64" min="64" style="0" width="8.08235294117647"/>
+    <col collapsed="false" hidden="false" max="63" min="63" style="0" width="10.2705882352941"/>
+    <col collapsed="false" hidden="false" max="64" min="64" style="0" width="8.09019607843137"/>
     <col collapsed="false" hidden="false" max="65" min="65" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="66" min="66" style="0" width="11.6078431372549"/>
+    <col collapsed="false" hidden="false" max="66" min="66" style="0" width="11.6196078431373"/>
     <col collapsed="false" hidden="false" max="67" min="67" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="68" min="68" style="0" width="13.956862745098"/>
-    <col collapsed="false" hidden="false" max="69" min="69" style="0" width="8.08235294117647"/>
+    <col collapsed="false" hidden="false" max="68" min="68" style="0" width="13.9647058823529"/>
+    <col collapsed="false" hidden="false" max="69" min="69" style="0" width="8.09019607843137"/>
     <col collapsed="false" hidden="false" max="70" min="70" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="71" min="71" style="0" width="11.6078431372549"/>
+    <col collapsed="false" hidden="false" max="71" min="71" style="0" width="11.6196078431373"/>
     <col collapsed="false" hidden="false" max="72" min="72" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="73" min="73" style="0" width="12.9450980392157"/>
-    <col collapsed="false" hidden="false" max="74" min="74" style="0" width="8.08235294117647"/>
+    <col collapsed="false" hidden="false" max="73" min="73" style="0" width="12.9529411764706"/>
+    <col collapsed="false" hidden="false" max="74" min="74" style="0" width="8.09019607843137"/>
     <col collapsed="false" hidden="false" max="75" min="75" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="76" min="76" style="0" width="11.6078431372549"/>
+    <col collapsed="false" hidden="false" max="76" min="76" style="0" width="11.6196078431373"/>
     <col collapsed="false" hidden="false" max="77" min="77" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="78" min="78" style="0" width="12.7764705882353"/>
-    <col collapsed="false" hidden="false" max="79" min="79" style="0" width="8.08235294117647"/>
+    <col collapsed="false" hidden="false" max="78" min="78" style="0" width="12.7882352941176"/>
+    <col collapsed="false" hidden="false" max="79" min="79" style="0" width="8.09019607843137"/>
     <col collapsed="false" hidden="false" max="80" min="80" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="81" min="81" style="0" width="11.6078431372549"/>
+    <col collapsed="false" hidden="false" max="81" min="81" style="0" width="11.6196078431373"/>
     <col collapsed="false" hidden="false" max="82" min="82" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="83" min="83" style="0" width="13.6352941176471"/>
-    <col collapsed="false" hidden="false" max="84" min="84" style="0" width="8.08235294117647"/>
+    <col collapsed="false" hidden="false" max="83" min="83" style="0" width="13.643137254902"/>
+    <col collapsed="false" hidden="false" max="84" min="84" style="0" width="8.09019607843137"/>
     <col collapsed="false" hidden="false" max="85" min="85" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="86" min="86" style="0" width="11.6078431372549"/>
+    <col collapsed="false" hidden="false" max="86" min="86" style="0" width="11.6196078431373"/>
     <col collapsed="false" hidden="false" max="87" min="87" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="88" min="88" style="0" width="14.7960784313726"/>
-    <col collapsed="false" hidden="false" max="89" min="89" style="0" width="8.08235294117647"/>
+    <col collapsed="false" hidden="false" max="88" min="88" style="0" width="14.8039215686275"/>
+    <col collapsed="false" hidden="false" max="89" min="89" style="0" width="8.09019607843137"/>
     <col collapsed="false" hidden="false" max="90" min="90" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="91" min="91" style="0" width="11.6078431372549"/>
+    <col collapsed="false" hidden="false" max="91" min="91" style="0" width="11.6196078431373"/>
     <col collapsed="false" hidden="false" max="92" min="92" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="93" min="93" style="0" width="10.2627450980392"/>
-    <col collapsed="false" hidden="false" max="94" min="94" style="0" width="13.7921568627451"/>
-    <col collapsed="false" hidden="false" max="95" min="95" style="0" width="14.7960784313726"/>
-    <col collapsed="false" hidden="false" max="96" min="96" style="0" width="17.321568627451"/>
+    <col collapsed="false" hidden="false" max="93" min="93" style="0" width="10.2705882352941"/>
+    <col collapsed="false" hidden="false" max="94" min="94" style="0" width="13.8"/>
+    <col collapsed="false" hidden="false" max="95" min="95" style="0" width="14.8039215686275"/>
+    <col collapsed="false" hidden="false" max="96" min="96" style="0" width="17.3372549019608"/>
     <col collapsed="false" hidden="false" max="97" min="97" style="0" width="6.02352941176471"/>
-    <col collapsed="false" hidden="false" max="98" min="98" style="0" width="23.0313725490196"/>
-    <col collapsed="false" hidden="false" max="99" min="99" style="0" width="15.9764705882353"/>
-    <col collapsed="false" hidden="false" max="100" min="100" style="0" width="17.1529411764706"/>
-    <col collapsed="false" hidden="false" max="101" min="101" style="0" width="17.321568627451"/>
+    <col collapsed="false" hidden="false" max="98" min="98" style="0" width="23.043137254902"/>
+    <col collapsed="false" hidden="false" max="99" min="99" style="0" width="15.9921568627451"/>
+    <col collapsed="false" hidden="false" max="100" min="100" style="0" width="17.1647058823529"/>
+    <col collapsed="false" hidden="false" max="101" min="101" style="0" width="17.3372549019608"/>
     <col collapsed="false" hidden="false" max="102" min="102" style="0" width="6.02352941176471"/>
-    <col collapsed="false" hidden="false" max="103" min="103" style="0" width="22.1960784313725"/>
-    <col collapsed="false" hidden="false" max="104" min="104" style="0" width="15.9764705882353"/>
-    <col collapsed="false" hidden="false" max="105" min="105" style="0" width="17.1529411764706"/>
-    <col collapsed="false" hidden="false" max="106" min="106" style="0" width="17.321568627451"/>
+    <col collapsed="false" hidden="false" max="103" min="103" style="0" width="22.2117647058824"/>
+    <col collapsed="false" hidden="false" max="104" min="104" style="0" width="15.9921568627451"/>
+    <col collapsed="false" hidden="false" max="105" min="105" style="0" width="17.1647058823529"/>
+    <col collapsed="false" hidden="false" max="106" min="106" style="0" width="17.3372549019608"/>
     <col collapsed="false" hidden="false" max="107" min="107" style="0" width="6.02352941176471"/>
-    <col collapsed="false" hidden="false" max="108" min="108" style="0" width="11.7725490196078"/>
-    <col collapsed="false" hidden="false" max="109" min="109" style="0" width="17.321568627451"/>
-    <col collapsed="false" hidden="false" max="110" min="110" style="0" width="12.7764705882353"/>
-    <col collapsed="false" hidden="false" max="111" min="111" style="0" width="18.5098039215686"/>
-    <col collapsed="false" hidden="false" max="112" min="112" style="0" width="17.321568627451"/>
-    <col collapsed="false" hidden="false" max="113" min="113" style="0" width="12.7764705882353"/>
-    <col collapsed="false" hidden="false" max="114" min="114" style="0" width="19.5137254901961"/>
-    <col collapsed="false" hidden="false" max="115" min="115" style="0" width="17.321568627451"/>
-    <col collapsed="false" hidden="false" max="116" min="116" style="0" width="12.7764705882353"/>
-    <col collapsed="false" hidden="false" max="117" min="117" style="0" width="18.6823529411765"/>
-    <col collapsed="false" hidden="false" max="119" min="118" style="0" width="17.321568627451"/>
-    <col collapsed="false" hidden="false" max="120" min="120" style="0" width="16.4823529411765"/>
-    <col collapsed="false" hidden="false" max="121" min="121" style="0" width="11.7725490196078"/>
-    <col collapsed="false" hidden="false" max="122" min="122" style="0" width="15.6509803921569"/>
-    <col collapsed="false" hidden="false" max="123" min="123" style="0" width="16.3176470588235"/>
-    <col collapsed="false" hidden="false" max="124" min="124" style="0" width="18.5098039215686"/>
-    <col collapsed="false" hidden="false" max="125" min="125" style="0" width="14.4627450980392"/>
-    <col collapsed="false" hidden="false" max="126" min="126" style="0" width="13.6352941176471"/>
-    <col collapsed="false" hidden="false" max="138" min="127" style="0" width="18.6823529411765"/>
-    <col collapsed="false" hidden="false" max="140" min="139" style="0" width="30.9490196078431"/>
-    <col collapsed="false" hidden="false" max="141" min="141" style="0" width="26.0823529411765"/>
-    <col collapsed="false" hidden="false" max="142" min="142" style="0" width="20.6941176470588"/>
-    <col collapsed="false" hidden="false" max="143" min="143" style="0" width="13.1098039215686"/>
+    <col collapsed="false" hidden="false" max="108" min="108" style="0" width="11.7764705882353"/>
+    <col collapsed="false" hidden="false" max="109" min="109" style="0" width="17.3372549019608"/>
+    <col collapsed="false" hidden="false" max="110" min="110" style="0" width="12.7882352941176"/>
+    <col collapsed="false" hidden="false" max="111" min="111" style="0" width="18.521568627451"/>
+    <col collapsed="false" hidden="false" max="112" min="112" style="0" width="17.3372549019608"/>
+    <col collapsed="false" hidden="false" max="113" min="113" style="0" width="12.7882352941176"/>
+    <col collapsed="false" hidden="false" max="114" min="114" style="0" width="19.5254901960784"/>
+    <col collapsed="false" hidden="false" max="115" min="115" style="0" width="17.3372549019608"/>
+    <col collapsed="false" hidden="false" max="116" min="116" style="0" width="12.7882352941176"/>
+    <col collapsed="false" hidden="false" max="117" min="117" style="0" width="18.6941176470588"/>
+    <col collapsed="false" hidden="false" max="119" min="118" style="0" width="17.3372549019608"/>
+    <col collapsed="false" hidden="false" max="120" min="120" style="0" width="16.4941176470588"/>
+    <col collapsed="false" hidden="false" max="121" min="121" style="0" width="11.7764705882353"/>
+    <col collapsed="false" hidden="false" max="122" min="122" style="0" width="15.6627450980392"/>
+    <col collapsed="false" hidden="false" max="123" min="123" style="0" width="16.3254901960784"/>
+    <col collapsed="false" hidden="false" max="124" min="124" style="0" width="18.521568627451"/>
+    <col collapsed="false" hidden="false" max="125" min="125" style="0" width="14.4666666666667"/>
+    <col collapsed="false" hidden="false" max="126" min="126" style="0" width="13.643137254902"/>
+    <col collapsed="false" hidden="false" max="138" min="127" style="0" width="18.6941176470588"/>
+    <col collapsed="false" hidden="false" max="140" min="139" style="0" width="30.9725490196078"/>
+    <col collapsed="false" hidden="false" max="141" min="141" style="0" width="26.1019607843137"/>
+    <col collapsed="false" hidden="false" max="142" min="142" style="0" width="20.7098039215686"/>
+    <col collapsed="false" hidden="false" max="143" min="143" style="0" width="13.121568627451"/>
     <col collapsed="false" hidden="false" max="144" min="144" style="0" width="7.74117647058824"/>
-    <col collapsed="false" hidden="false" max="145" min="145" style="0" width="13.4509803921569"/>
-    <col collapsed="false" hidden="false" max="146" min="146" style="0" width="10.4274509803922"/>
-    <col collapsed="false" hidden="false" max="1025" min="147" style="0" width="18.6823529411765"/>
+    <col collapsed="false" hidden="false" max="145" min="145" style="0" width="13.4588235294118"/>
+    <col collapsed="false" hidden="false" max="146" min="146" style="0" width="10.4313725490196"/>
+    <col collapsed="false" hidden="false" max="1025" min="147" style="0" width="18.6941176470588"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="1">
@@ -12389,140 +12389,140 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.0862745098039"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.2627450980392"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.92156862745098"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.0039215686275"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.9137254901961"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.4666666666667"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.3921568627451"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.4470588235294"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.6509803921569"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="18.6823529411765"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="15.3098039215686"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.6039215686275"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="11.9411764705882"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="13.7921568627451"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="12.9450980392157"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.956862745098"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="16.4823529411765"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.2705882352941"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="16.3176470588235"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="13.956862745098"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="10.2627450980392"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="10.7607843137255"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="8.08235294117647"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.1058823529412"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.2705882352941"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.92941176470588"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.0196078431373"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.9333333333333"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.478431372549"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.4039215686274"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.4549019607843"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.6627450980392"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="18.6941176470588"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="15.321568627451"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.6117647058824"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="11.9490196078431"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="13.8"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="12.9529411764706"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.9647058823529"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="16.4941176470588"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.278431372549"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="16.3254901960784"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="13.9647058823529"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="10.2705882352941"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="10.7686274509804"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="8.09019607843137"/>
     <col collapsed="false" hidden="false" max="24" min="24" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="11.6078431372549"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="11.6196078431373"/>
     <col collapsed="false" hidden="false" max="26" min="26" style="0" width="5.52549019607843"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="11.6078431372549"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="14.1254901960784"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="10.7607843137255"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="8.08235294117647"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="11.6196078431373"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="14.1333333333333"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="10.7686274509804"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="8.09019607843137"/>
     <col collapsed="false" hidden="false" max="31" min="31" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="11.6078431372549"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="11.6196078431373"/>
     <col collapsed="false" hidden="false" max="33" min="33" style="0" width="5.52549019607843"/>
     <col collapsed="false" hidden="false" max="34" min="34" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="14.6392156862745"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="10.7607843137255"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="8.08235294117647"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="14.6509803921569"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="10.7686274509804"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="8.09019607843137"/>
     <col collapsed="false" hidden="false" max="38" min="38" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="11.6078431372549"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="11.6196078431373"/>
     <col collapsed="false" hidden="false" max="40" min="40" style="0" width="5.52549019607843"/>
     <col collapsed="false" hidden="false" max="41" min="41" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="14.2980392156863"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="10.7607843137255"/>
-    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="8.08235294117647"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="14.3058823529412"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="10.7686274509804"/>
+    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="8.09019607843137"/>
     <col collapsed="false" hidden="false" max="45" min="45" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="11.6078431372549"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="11.6196078431373"/>
     <col collapsed="false" hidden="false" max="47" min="47" style="0" width="5.52549019607843"/>
     <col collapsed="false" hidden="false" max="48" min="48" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="49" min="49" style="0" width="14.7960784313726"/>
-    <col collapsed="false" hidden="false" max="50" min="50" style="0" width="10.7607843137255"/>
-    <col collapsed="false" hidden="false" max="51" min="51" style="0" width="8.08235294117647"/>
+    <col collapsed="false" hidden="false" max="49" min="49" style="0" width="14.8039215686275"/>
+    <col collapsed="false" hidden="false" max="50" min="50" style="0" width="10.7686274509804"/>
+    <col collapsed="false" hidden="false" max="51" min="51" style="0" width="8.09019607843137"/>
     <col collapsed="false" hidden="false" max="52" min="52" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="53" min="53" style="0" width="11.6078431372549"/>
+    <col collapsed="false" hidden="false" max="53" min="53" style="0" width="11.6196078431373"/>
     <col collapsed="false" hidden="false" max="54" min="54" style="0" width="5.52549019607843"/>
     <col collapsed="false" hidden="false" max="55" min="55" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="56" min="56" style="0" width="15.1372549019608"/>
-    <col collapsed="false" hidden="false" max="57" min="57" style="0" width="10.7607843137255"/>
-    <col collapsed="false" hidden="false" max="58" min="58" style="0" width="8.08235294117647"/>
+    <col collapsed="false" hidden="false" max="56" min="56" style="0" width="15.1490196078431"/>
+    <col collapsed="false" hidden="false" max="57" min="57" style="0" width="10.7686274509804"/>
+    <col collapsed="false" hidden="false" max="58" min="58" style="0" width="8.09019607843137"/>
     <col collapsed="false" hidden="false" max="59" min="59" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="60" min="60" style="0" width="11.6078431372549"/>
+    <col collapsed="false" hidden="false" max="60" min="60" style="0" width="11.6196078431373"/>
     <col collapsed="false" hidden="false" max="61" min="61" style="0" width="5.52549019607843"/>
     <col collapsed="false" hidden="false" max="62" min="62" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="63" min="63" style="0" width="10.2627450980392"/>
-    <col collapsed="false" hidden="false" max="64" min="64" style="0" width="8.08235294117647"/>
+    <col collapsed="false" hidden="false" max="63" min="63" style="0" width="10.2705882352941"/>
+    <col collapsed="false" hidden="false" max="64" min="64" style="0" width="8.09019607843137"/>
     <col collapsed="false" hidden="false" max="65" min="65" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="66" min="66" style="0" width="11.6078431372549"/>
+    <col collapsed="false" hidden="false" max="66" min="66" style="0" width="11.6196078431373"/>
     <col collapsed="false" hidden="false" max="67" min="67" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="68" min="68" style="0" width="13.956862745098"/>
-    <col collapsed="false" hidden="false" max="69" min="69" style="0" width="8.08235294117647"/>
+    <col collapsed="false" hidden="false" max="68" min="68" style="0" width="13.9647058823529"/>
+    <col collapsed="false" hidden="false" max="69" min="69" style="0" width="8.09019607843137"/>
     <col collapsed="false" hidden="false" max="70" min="70" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="71" min="71" style="0" width="11.6078431372549"/>
+    <col collapsed="false" hidden="false" max="71" min="71" style="0" width="11.6196078431373"/>
     <col collapsed="false" hidden="false" max="72" min="72" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="73" min="73" style="0" width="12.9450980392157"/>
-    <col collapsed="false" hidden="false" max="74" min="74" style="0" width="8.08235294117647"/>
+    <col collapsed="false" hidden="false" max="73" min="73" style="0" width="12.9529411764706"/>
+    <col collapsed="false" hidden="false" max="74" min="74" style="0" width="8.09019607843137"/>
     <col collapsed="false" hidden="false" max="75" min="75" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="76" min="76" style="0" width="11.6078431372549"/>
+    <col collapsed="false" hidden="false" max="76" min="76" style="0" width="11.6196078431373"/>
     <col collapsed="false" hidden="false" max="77" min="77" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="78" min="78" style="0" width="12.7764705882353"/>
-    <col collapsed="false" hidden="false" max="79" min="79" style="0" width="8.08235294117647"/>
+    <col collapsed="false" hidden="false" max="78" min="78" style="0" width="12.7882352941176"/>
+    <col collapsed="false" hidden="false" max="79" min="79" style="0" width="8.09019607843137"/>
     <col collapsed="false" hidden="false" max="80" min="80" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="81" min="81" style="0" width="11.6078431372549"/>
+    <col collapsed="false" hidden="false" max="81" min="81" style="0" width="11.6196078431373"/>
     <col collapsed="false" hidden="false" max="82" min="82" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="83" min="83" style="0" width="13.6352941176471"/>
-    <col collapsed="false" hidden="false" max="84" min="84" style="0" width="8.08235294117647"/>
+    <col collapsed="false" hidden="false" max="83" min="83" style="0" width="13.643137254902"/>
+    <col collapsed="false" hidden="false" max="84" min="84" style="0" width="8.09019607843137"/>
     <col collapsed="false" hidden="false" max="85" min="85" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="86" min="86" style="0" width="11.6078431372549"/>
+    <col collapsed="false" hidden="false" max="86" min="86" style="0" width="11.6196078431373"/>
     <col collapsed="false" hidden="false" max="87" min="87" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="88" min="88" style="0" width="14.7960784313726"/>
-    <col collapsed="false" hidden="false" max="89" min="89" style="0" width="8.08235294117647"/>
+    <col collapsed="false" hidden="false" max="88" min="88" style="0" width="14.8039215686275"/>
+    <col collapsed="false" hidden="false" max="89" min="89" style="0" width="8.09019607843137"/>
     <col collapsed="false" hidden="false" max="90" min="90" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="91" min="91" style="0" width="11.6078431372549"/>
+    <col collapsed="false" hidden="false" max="91" min="91" style="0" width="11.6196078431373"/>
     <col collapsed="false" hidden="false" max="92" min="92" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="93" min="93" style="0" width="10.2627450980392"/>
-    <col collapsed="false" hidden="false" max="94" min="94" style="0" width="13.7921568627451"/>
-    <col collapsed="false" hidden="false" max="95" min="95" style="0" width="14.7960784313726"/>
-    <col collapsed="false" hidden="false" max="96" min="96" style="0" width="17.321568627451"/>
+    <col collapsed="false" hidden="false" max="93" min="93" style="0" width="10.2705882352941"/>
+    <col collapsed="false" hidden="false" max="94" min="94" style="0" width="13.8"/>
+    <col collapsed="false" hidden="false" max="95" min="95" style="0" width="14.8039215686275"/>
+    <col collapsed="false" hidden="false" max="96" min="96" style="0" width="17.3372549019608"/>
     <col collapsed="false" hidden="false" max="97" min="97" style="0" width="6.02352941176471"/>
-    <col collapsed="false" hidden="false" max="98" min="98" style="0" width="23.0313725490196"/>
-    <col collapsed="false" hidden="false" max="99" min="99" style="0" width="15.9764705882353"/>
-    <col collapsed="false" hidden="false" max="100" min="100" style="0" width="17.1529411764706"/>
-    <col collapsed="false" hidden="false" max="101" min="101" style="0" width="17.321568627451"/>
+    <col collapsed="false" hidden="false" max="98" min="98" style="0" width="23.043137254902"/>
+    <col collapsed="false" hidden="false" max="99" min="99" style="0" width="15.9921568627451"/>
+    <col collapsed="false" hidden="false" max="100" min="100" style="0" width="17.1647058823529"/>
+    <col collapsed="false" hidden="false" max="101" min="101" style="0" width="17.3372549019608"/>
     <col collapsed="false" hidden="false" max="102" min="102" style="0" width="6.02352941176471"/>
-    <col collapsed="false" hidden="false" max="103" min="103" style="0" width="22.1960784313725"/>
-    <col collapsed="false" hidden="false" max="104" min="104" style="0" width="15.9764705882353"/>
-    <col collapsed="false" hidden="false" max="105" min="105" style="0" width="17.1529411764706"/>
-    <col collapsed="false" hidden="false" max="106" min="106" style="0" width="17.321568627451"/>
+    <col collapsed="false" hidden="false" max="103" min="103" style="0" width="22.2117647058824"/>
+    <col collapsed="false" hidden="false" max="104" min="104" style="0" width="15.9921568627451"/>
+    <col collapsed="false" hidden="false" max="105" min="105" style="0" width="17.1647058823529"/>
+    <col collapsed="false" hidden="false" max="106" min="106" style="0" width="17.3372549019608"/>
     <col collapsed="false" hidden="false" max="107" min="107" style="0" width="6.02352941176471"/>
-    <col collapsed="false" hidden="false" max="108" min="108" style="0" width="11.7725490196078"/>
-    <col collapsed="false" hidden="false" max="109" min="109" style="0" width="17.321568627451"/>
-    <col collapsed="false" hidden="false" max="110" min="110" style="0" width="12.7764705882353"/>
-    <col collapsed="false" hidden="false" max="111" min="111" style="0" width="18.5098039215686"/>
-    <col collapsed="false" hidden="false" max="112" min="112" style="0" width="17.321568627451"/>
-    <col collapsed="false" hidden="false" max="113" min="113" style="0" width="12.7764705882353"/>
-    <col collapsed="false" hidden="false" max="114" min="114" style="0" width="19.5137254901961"/>
-    <col collapsed="false" hidden="false" max="115" min="115" style="0" width="17.321568627451"/>
-    <col collapsed="false" hidden="false" max="116" min="116" style="0" width="12.7764705882353"/>
-    <col collapsed="false" hidden="false" max="117" min="117" style="0" width="18.6823529411765"/>
-    <col collapsed="false" hidden="false" max="119" min="118" style="0" width="17.321568627451"/>
-    <col collapsed="false" hidden="false" max="120" min="120" style="0" width="16.4823529411765"/>
-    <col collapsed="false" hidden="false" max="121" min="121" style="0" width="11.7725490196078"/>
-    <col collapsed="false" hidden="false" max="122" min="122" style="0" width="15.6509803921569"/>
-    <col collapsed="false" hidden="false" max="123" min="123" style="0" width="16.3176470588235"/>
-    <col collapsed="false" hidden="false" max="124" min="124" style="0" width="18.5098039215686"/>
-    <col collapsed="false" hidden="false" max="125" min="125" style="0" width="14.4627450980392"/>
-    <col collapsed="false" hidden="false" max="126" min="126" style="0" width="13.6352941176471"/>
-    <col collapsed="false" hidden="false" max="138" min="127" style="0" width="18.6823529411765"/>
-    <col collapsed="false" hidden="false" max="140" min="139" style="0" width="30.9490196078431"/>
-    <col collapsed="false" hidden="false" max="141" min="141" style="0" width="26.0823529411765"/>
-    <col collapsed="false" hidden="false" max="142" min="142" style="0" width="20.6941176470588"/>
-    <col collapsed="false" hidden="false" max="143" min="143" style="0" width="13.1098039215686"/>
+    <col collapsed="false" hidden="false" max="108" min="108" style="0" width="11.7764705882353"/>
+    <col collapsed="false" hidden="false" max="109" min="109" style="0" width="17.3372549019608"/>
+    <col collapsed="false" hidden="false" max="110" min="110" style="0" width="12.7882352941176"/>
+    <col collapsed="false" hidden="false" max="111" min="111" style="0" width="18.521568627451"/>
+    <col collapsed="false" hidden="false" max="112" min="112" style="0" width="17.3372549019608"/>
+    <col collapsed="false" hidden="false" max="113" min="113" style="0" width="12.7882352941176"/>
+    <col collapsed="false" hidden="false" max="114" min="114" style="0" width="19.5254901960784"/>
+    <col collapsed="false" hidden="false" max="115" min="115" style="0" width="17.3372549019608"/>
+    <col collapsed="false" hidden="false" max="116" min="116" style="0" width="12.7882352941176"/>
+    <col collapsed="false" hidden="false" max="117" min="117" style="0" width="18.6941176470588"/>
+    <col collapsed="false" hidden="false" max="119" min="118" style="0" width="17.3372549019608"/>
+    <col collapsed="false" hidden="false" max="120" min="120" style="0" width="16.4941176470588"/>
+    <col collapsed="false" hidden="false" max="121" min="121" style="0" width="11.7764705882353"/>
+    <col collapsed="false" hidden="false" max="122" min="122" style="0" width="15.6627450980392"/>
+    <col collapsed="false" hidden="false" max="123" min="123" style="0" width="16.3254901960784"/>
+    <col collapsed="false" hidden="false" max="124" min="124" style="0" width="18.521568627451"/>
+    <col collapsed="false" hidden="false" max="125" min="125" style="0" width="14.4666666666667"/>
+    <col collapsed="false" hidden="false" max="126" min="126" style="0" width="13.643137254902"/>
+    <col collapsed="false" hidden="false" max="138" min="127" style="0" width="18.6941176470588"/>
+    <col collapsed="false" hidden="false" max="140" min="139" style="0" width="30.9725490196078"/>
+    <col collapsed="false" hidden="false" max="141" min="141" style="0" width="26.1019607843137"/>
+    <col collapsed="false" hidden="false" max="142" min="142" style="0" width="20.7098039215686"/>
+    <col collapsed="false" hidden="false" max="143" min="143" style="0" width="13.121568627451"/>
     <col collapsed="false" hidden="false" max="144" min="144" style="0" width="7.74117647058824"/>
-    <col collapsed="false" hidden="false" max="145" min="145" style="0" width="13.4509803921569"/>
-    <col collapsed="false" hidden="false" max="146" min="146" style="0" width="10.4274509803922"/>
-    <col collapsed="false" hidden="false" max="1025" min="147" style="0" width="18.6823529411765"/>
+    <col collapsed="false" hidden="false" max="145" min="145" style="0" width="13.4588235294118"/>
+    <col collapsed="false" hidden="false" max="146" min="146" style="0" width="10.4313725490196"/>
+    <col collapsed="false" hidden="false" max="1025" min="147" style="0" width="18.6941176470588"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="1">

</xml_diff>

<commit_message>
most important executive validations implemented
</commit_message>
<xml_diff>
--- a/core/test/input/FullValuesOnly.xlsx
+++ b/core/test/input/FullValuesOnly.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="245" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="3" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="245" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="DOC_SRC" sheetId="1" state="visible" r:id="rId2"/>
@@ -1168,17 +1168,17 @@
   </sheetPr>
   <dimension ref="A1:T68"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A40" view="normal" windowProtection="false" workbookViewId="0" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100">
-      <selection activeCell="C56" activeCellId="0" pane="topLeft" sqref="C56"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A31" view="normal" windowProtection="false" workbookViewId="0" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100">
+      <selection activeCell="B42" activeCellId="0" pane="topLeft" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.6549019607843"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.9019607843137"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.043137254902"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.2196078431373"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.5333333333333"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.7607843137255"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.6627450980392"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.9176470588235"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.0627450980392"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.2392156862745"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.5450980392157"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.7686274509804"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="1">
@@ -2644,145 +2644,145 @@
   </sheetPr>
   <dimension ref="A1:EP32"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="CD1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="DS1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100">
       <selection activeCell="DV4" activeCellId="0" pane="topLeft" sqref="DV4"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.1058823529412"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.2705882352941"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.92941176470588"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.0196078431373"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.9333333333333"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.478431372549"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.4039215686274"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.4549019607843"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.6627450980392"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="18.6941176470588"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="15.321568627451"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.6117647058824"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="11.9490196078431"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="13.8"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="12.9529411764706"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.9647058823529"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="16.4941176470588"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.278431372549"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="16.3254901960784"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="13.9647058823529"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="10.2705882352941"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="10.7686274509804"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="8.09019607843137"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.1176470588235"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.2745098039216"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.93333333333333"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.0313725490196"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.9490196078431"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.4901960784314"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.4196078431373"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.4588235294118"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.6705882352941"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="18.7058823529412"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="15.3333333333333"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.6235294117647"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="11.956862745098"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="13.8039215686275"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="12.9607843137255"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.9764705882353"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="16.5019607843137"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.2901960784314"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="16.3372549019608"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="13.9764705882353"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="10.2745098039216"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="10.7725490196078"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="8.09803921568627"/>
     <col collapsed="false" hidden="false" max="24" min="24" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="11.6196078431373"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="11.6274509803922"/>
     <col collapsed="false" hidden="false" max="26" min="26" style="0" width="5.52549019607843"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="11.6196078431373"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="14.1333333333333"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="10.7686274509804"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="8.09019607843137"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="11.6274509803922"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="14.1411764705882"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="10.7725490196078"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="8.09803921568627"/>
     <col collapsed="false" hidden="false" max="31" min="31" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="11.6196078431373"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="11.6274509803922"/>
     <col collapsed="false" hidden="false" max="33" min="33" style="0" width="5.52549019607843"/>
     <col collapsed="false" hidden="false" max="34" min="34" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="14.6509803921569"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="10.7686274509804"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="8.09019607843137"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="14.6588235294118"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="10.7725490196078"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="8.09803921568627"/>
     <col collapsed="false" hidden="false" max="38" min="38" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="11.6196078431373"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="11.6274509803922"/>
     <col collapsed="false" hidden="false" max="40" min="40" style="0" width="5.52549019607843"/>
     <col collapsed="false" hidden="false" max="41" min="41" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="14.3058823529412"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="10.7686274509804"/>
-    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="8.09019607843137"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="14.3176470588235"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="10.7725490196078"/>
+    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="8.09803921568627"/>
     <col collapsed="false" hidden="false" max="45" min="45" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="11.6196078431373"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="11.6274509803922"/>
     <col collapsed="false" hidden="false" max="47" min="47" style="0" width="5.52549019607843"/>
     <col collapsed="false" hidden="false" max="48" min="48" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="49" min="49" style="0" width="14.8039215686275"/>
-    <col collapsed="false" hidden="false" max="50" min="50" style="0" width="10.7686274509804"/>
-    <col collapsed="false" hidden="false" max="51" min="51" style="0" width="8.09019607843137"/>
+    <col collapsed="false" hidden="false" max="49" min="49" style="0" width="14.8156862745098"/>
+    <col collapsed="false" hidden="false" max="50" min="50" style="0" width="10.7725490196078"/>
+    <col collapsed="false" hidden="false" max="51" min="51" style="0" width="8.09803921568627"/>
     <col collapsed="false" hidden="false" max="52" min="52" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="53" min="53" style="0" width="11.6196078431373"/>
+    <col collapsed="false" hidden="false" max="53" min="53" style="0" width="11.6274509803922"/>
     <col collapsed="false" hidden="false" max="54" min="54" style="0" width="5.52549019607843"/>
     <col collapsed="false" hidden="false" max="55" min="55" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="56" min="56" style="0" width="15.1490196078431"/>
-    <col collapsed="false" hidden="false" max="57" min="57" style="0" width="10.7686274509804"/>
-    <col collapsed="false" hidden="false" max="58" min="58" style="0" width="8.09019607843137"/>
+    <col collapsed="false" hidden="false" max="56" min="56" style="0" width="15.156862745098"/>
+    <col collapsed="false" hidden="false" max="57" min="57" style="0" width="10.7725490196078"/>
+    <col collapsed="false" hidden="false" max="58" min="58" style="0" width="8.09803921568627"/>
     <col collapsed="false" hidden="false" max="59" min="59" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="60" min="60" style="0" width="11.6196078431373"/>
+    <col collapsed="false" hidden="false" max="60" min="60" style="0" width="11.6274509803922"/>
     <col collapsed="false" hidden="false" max="61" min="61" style="0" width="5.52549019607843"/>
     <col collapsed="false" hidden="false" max="62" min="62" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="63" min="63" style="0" width="10.2705882352941"/>
-    <col collapsed="false" hidden="false" max="64" min="64" style="0" width="8.09019607843137"/>
+    <col collapsed="false" hidden="false" max="63" min="63" style="0" width="10.2745098039216"/>
+    <col collapsed="false" hidden="false" max="64" min="64" style="0" width="8.09803921568627"/>
     <col collapsed="false" hidden="false" max="65" min="65" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="66" min="66" style="0" width="11.6196078431373"/>
+    <col collapsed="false" hidden="false" max="66" min="66" style="0" width="11.6274509803922"/>
     <col collapsed="false" hidden="false" max="67" min="67" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="68" min="68" style="0" width="13.9647058823529"/>
-    <col collapsed="false" hidden="false" max="69" min="69" style="0" width="8.09019607843137"/>
+    <col collapsed="false" hidden="false" max="68" min="68" style="0" width="13.9764705882353"/>
+    <col collapsed="false" hidden="false" max="69" min="69" style="0" width="8.09803921568627"/>
     <col collapsed="false" hidden="false" max="70" min="70" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="71" min="71" style="0" width="11.6196078431373"/>
+    <col collapsed="false" hidden="false" max="71" min="71" style="0" width="11.6274509803922"/>
     <col collapsed="false" hidden="false" max="72" min="72" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="73" min="73" style="0" width="12.9529411764706"/>
-    <col collapsed="false" hidden="false" max="74" min="74" style="0" width="8.09019607843137"/>
+    <col collapsed="false" hidden="false" max="73" min="73" style="0" width="12.9607843137255"/>
+    <col collapsed="false" hidden="false" max="74" min="74" style="0" width="8.09803921568627"/>
     <col collapsed="false" hidden="false" max="75" min="75" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="76" min="76" style="0" width="11.6196078431373"/>
+    <col collapsed="false" hidden="false" max="76" min="76" style="0" width="11.6274509803922"/>
     <col collapsed="false" hidden="false" max="77" min="77" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="78" min="78" style="0" width="12.7882352941176"/>
-    <col collapsed="false" hidden="false" max="79" min="79" style="0" width="8.09019607843137"/>
+    <col collapsed="false" hidden="false" max="78" min="78" style="0" width="12.7960784313726"/>
+    <col collapsed="false" hidden="false" max="79" min="79" style="0" width="8.09803921568627"/>
     <col collapsed="false" hidden="false" max="80" min="80" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="81" min="81" style="0" width="11.6196078431373"/>
+    <col collapsed="false" hidden="false" max="81" min="81" style="0" width="11.6274509803922"/>
     <col collapsed="false" hidden="false" max="82" min="82" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="83" min="83" style="0" width="13.643137254902"/>
-    <col collapsed="false" hidden="false" max="84" min="84" style="0" width="8.09019607843137"/>
+    <col collapsed="false" hidden="false" max="83" min="83" style="0" width="13.6549019607843"/>
+    <col collapsed="false" hidden="false" max="84" min="84" style="0" width="8.09803921568627"/>
     <col collapsed="false" hidden="false" max="85" min="85" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="86" min="86" style="0" width="11.6196078431373"/>
+    <col collapsed="false" hidden="false" max="86" min="86" style="0" width="11.6274509803922"/>
     <col collapsed="false" hidden="false" max="87" min="87" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="88" min="88" style="0" width="14.8039215686275"/>
-    <col collapsed="false" hidden="false" max="89" min="89" style="0" width="8.09019607843137"/>
+    <col collapsed="false" hidden="false" max="88" min="88" style="0" width="14.8156862745098"/>
+    <col collapsed="false" hidden="false" max="89" min="89" style="0" width="8.09803921568627"/>
     <col collapsed="false" hidden="false" max="90" min="90" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="91" min="91" style="0" width="11.6196078431373"/>
+    <col collapsed="false" hidden="false" max="91" min="91" style="0" width="11.6274509803922"/>
     <col collapsed="false" hidden="false" max="92" min="92" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="93" min="93" style="0" width="10.2705882352941"/>
-    <col collapsed="false" hidden="false" max="94" min="94" style="0" width="13.8"/>
-    <col collapsed="false" hidden="false" max="95" min="95" style="0" width="14.8039215686275"/>
-    <col collapsed="false" hidden="false" max="96" min="96" style="0" width="17.3372549019608"/>
+    <col collapsed="false" hidden="false" max="93" min="93" style="0" width="10.2745098039216"/>
+    <col collapsed="false" hidden="false" max="94" min="94" style="0" width="13.8039215686275"/>
+    <col collapsed="false" hidden="false" max="95" min="95" style="0" width="14.8156862745098"/>
+    <col collapsed="false" hidden="false" max="96" min="96" style="0" width="17.3490196078431"/>
     <col collapsed="false" hidden="false" max="97" min="97" style="0" width="6.02352941176471"/>
-    <col collapsed="false" hidden="false" max="98" min="98" style="0" width="23.043137254902"/>
-    <col collapsed="false" hidden="false" max="99" min="99" style="0" width="15.9921568627451"/>
-    <col collapsed="false" hidden="false" max="100" min="100" style="0" width="17.1647058823529"/>
-    <col collapsed="false" hidden="false" max="101" min="101" style="0" width="17.3372549019608"/>
+    <col collapsed="false" hidden="false" max="98" min="98" style="0" width="23.0588235294118"/>
+    <col collapsed="false" hidden="false" max="99" min="99" style="0" width="16.0039215686275"/>
+    <col collapsed="false" hidden="false" max="100" min="100" style="0" width="17.1764705882353"/>
+    <col collapsed="false" hidden="false" max="101" min="101" style="0" width="17.3490196078431"/>
     <col collapsed="false" hidden="false" max="102" min="102" style="0" width="6.02352941176471"/>
-    <col collapsed="false" hidden="false" max="103" min="103" style="0" width="22.2117647058824"/>
-    <col collapsed="false" hidden="false" max="104" min="104" style="0" width="15.9921568627451"/>
-    <col collapsed="false" hidden="false" max="105" min="105" style="0" width="17.1647058823529"/>
-    <col collapsed="false" hidden="false" max="106" min="106" style="0" width="17.3372549019608"/>
+    <col collapsed="false" hidden="false" max="103" min="103" style="0" width="22.2235294117647"/>
+    <col collapsed="false" hidden="false" max="104" min="104" style="0" width="16.0039215686275"/>
+    <col collapsed="false" hidden="false" max="105" min="105" style="0" width="17.1764705882353"/>
+    <col collapsed="false" hidden="false" max="106" min="106" style="0" width="17.3490196078431"/>
     <col collapsed="false" hidden="false" max="107" min="107" style="0" width="6.02352941176471"/>
-    <col collapsed="false" hidden="false" max="108" min="108" style="0" width="11.7764705882353"/>
-    <col collapsed="false" hidden="false" max="109" min="109" style="0" width="17.3372549019608"/>
-    <col collapsed="false" hidden="false" max="110" min="110" style="0" width="12.7882352941176"/>
-    <col collapsed="false" hidden="false" max="111" min="111" style="0" width="18.521568627451"/>
-    <col collapsed="false" hidden="false" max="112" min="112" style="0" width="17.3372549019608"/>
-    <col collapsed="false" hidden="false" max="113" min="113" style="0" width="12.7882352941176"/>
-    <col collapsed="false" hidden="false" max="114" min="114" style="0" width="19.5254901960784"/>
-    <col collapsed="false" hidden="false" max="115" min="115" style="0" width="17.3372549019608"/>
-    <col collapsed="false" hidden="false" max="116" min="116" style="0" width="12.7882352941176"/>
-    <col collapsed="false" hidden="false" max="117" min="117" style="0" width="18.6941176470588"/>
-    <col collapsed="false" hidden="false" max="119" min="118" style="0" width="17.3372549019608"/>
-    <col collapsed="false" hidden="false" max="120" min="120" style="0" width="16.4941176470588"/>
-    <col collapsed="false" hidden="false" max="121" min="121" style="0" width="11.7764705882353"/>
-    <col collapsed="false" hidden="false" max="122" min="122" style="0" width="15.6627450980392"/>
-    <col collapsed="false" hidden="false" max="123" min="123" style="0" width="16.3254901960784"/>
-    <col collapsed="false" hidden="false" max="124" min="124" style="0" width="18.521568627451"/>
-    <col collapsed="false" hidden="false" max="125" min="125" style="0" width="14.4666666666667"/>
-    <col collapsed="false" hidden="false" max="126" min="126" style="0" width="13.643137254902"/>
-    <col collapsed="false" hidden="false" max="138" min="127" style="0" width="18.6941176470588"/>
-    <col collapsed="false" hidden="false" max="140" min="139" style="0" width="30.9725490196078"/>
-    <col collapsed="false" hidden="false" max="141" min="141" style="0" width="26.1019607843137"/>
-    <col collapsed="false" hidden="false" max="142" min="142" style="0" width="20.7098039215686"/>
-    <col collapsed="false" hidden="false" max="143" min="143" style="0" width="13.121568627451"/>
+    <col collapsed="false" hidden="false" max="108" min="108" style="0" width="11.7843137254902"/>
+    <col collapsed="false" hidden="false" max="109" min="109" style="0" width="17.3490196078431"/>
+    <col collapsed="false" hidden="false" max="110" min="110" style="0" width="12.7960784313726"/>
+    <col collapsed="false" hidden="false" max="111" min="111" style="0" width="18.5294117647059"/>
+    <col collapsed="false" hidden="false" max="112" min="112" style="0" width="17.3490196078431"/>
+    <col collapsed="false" hidden="false" max="113" min="113" style="0" width="12.7960784313726"/>
+    <col collapsed="false" hidden="false" max="114" min="114" style="0" width="19.5411764705882"/>
+    <col collapsed="false" hidden="false" max="115" min="115" style="0" width="17.3490196078431"/>
+    <col collapsed="false" hidden="false" max="116" min="116" style="0" width="12.7960784313726"/>
+    <col collapsed="false" hidden="false" max="117" min="117" style="0" width="18.7058823529412"/>
+    <col collapsed="false" hidden="false" max="119" min="118" style="0" width="17.3490196078431"/>
+    <col collapsed="false" hidden="false" max="120" min="120" style="0" width="16.5019607843137"/>
+    <col collapsed="false" hidden="false" max="121" min="121" style="0" width="11.7843137254902"/>
+    <col collapsed="false" hidden="false" max="122" min="122" style="0" width="15.6705882352941"/>
+    <col collapsed="false" hidden="false" max="123" min="123" style="0" width="16.3372549019608"/>
+    <col collapsed="false" hidden="false" max="124" min="124" style="0" width="18.5294117647059"/>
+    <col collapsed="false" hidden="false" max="125" min="125" style="0" width="14.4745098039216"/>
+    <col collapsed="false" hidden="false" max="126" min="126" style="0" width="13.6549019607843"/>
+    <col collapsed="false" hidden="false" max="138" min="127" style="0" width="18.7058823529412"/>
+    <col collapsed="false" hidden="false" max="140" min="139" style="0" width="30.9960784313725"/>
+    <col collapsed="false" hidden="false" max="141" min="141" style="0" width="26.1137254901961"/>
+    <col collapsed="false" hidden="false" max="142" min="142" style="0" width="20.721568627451"/>
+    <col collapsed="false" hidden="false" max="143" min="143" style="0" width="13.1294117647059"/>
     <col collapsed="false" hidden="false" max="144" min="144" style="0" width="7.74117647058824"/>
-    <col collapsed="false" hidden="false" max="145" min="145" style="0" width="13.4588235294118"/>
-    <col collapsed="false" hidden="false" max="146" min="146" style="0" width="10.4313725490196"/>
-    <col collapsed="false" hidden="false" max="1025" min="147" style="0" width="18.6941176470588"/>
+    <col collapsed="false" hidden="false" max="145" min="145" style="0" width="13.4627450980392"/>
+    <col collapsed="false" hidden="false" max="146" min="146" style="0" width="10.4392156862745"/>
+    <col collapsed="false" hidden="false" max="1025" min="147" style="0" width="18.7058823529412"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="1">
@@ -7514,145 +7514,145 @@
   </sheetPr>
   <dimension ref="A1:EP32"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="I1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100">
+      <selection activeCell="L4" activeCellId="0" pane="topLeft" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.1058823529412"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.2705882352941"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.92941176470588"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.0196078431373"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.9333333333333"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.478431372549"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.4039215686274"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.4549019607843"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.6627450980392"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="18.6941176470588"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="15.321568627451"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.6117647058824"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="11.9490196078431"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="13.8"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="12.9529411764706"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.9647058823529"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="16.4941176470588"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.278431372549"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="16.3254901960784"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="13.9647058823529"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="10.2705882352941"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="10.7686274509804"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="8.09019607843137"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.1176470588235"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.2745098039216"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.93333333333333"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.0313725490196"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.9490196078431"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.4901960784314"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.4196078431373"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.4588235294118"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.6705882352941"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="18.7058823529412"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="15.3333333333333"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.6235294117647"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="11.956862745098"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="13.8039215686275"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="12.9607843137255"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.9764705882353"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="16.5019607843137"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.2901960784314"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="16.3372549019608"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="13.9764705882353"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="10.2745098039216"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="10.7725490196078"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="8.09803921568627"/>
     <col collapsed="false" hidden="false" max="24" min="24" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="11.6196078431373"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="11.6274509803922"/>
     <col collapsed="false" hidden="false" max="26" min="26" style="0" width="5.52549019607843"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="11.6196078431373"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="14.1333333333333"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="10.7686274509804"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="8.09019607843137"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="11.6274509803922"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="14.1411764705882"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="10.7725490196078"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="8.09803921568627"/>
     <col collapsed="false" hidden="false" max="31" min="31" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="11.6196078431373"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="11.6274509803922"/>
     <col collapsed="false" hidden="false" max="33" min="33" style="0" width="5.52549019607843"/>
     <col collapsed="false" hidden="false" max="34" min="34" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="14.6509803921569"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="10.7686274509804"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="8.09019607843137"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="14.6588235294118"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="10.7725490196078"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="8.09803921568627"/>
     <col collapsed="false" hidden="false" max="38" min="38" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="11.6196078431373"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="11.6274509803922"/>
     <col collapsed="false" hidden="false" max="40" min="40" style="0" width="5.52549019607843"/>
     <col collapsed="false" hidden="false" max="41" min="41" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="14.3058823529412"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="10.7686274509804"/>
-    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="8.09019607843137"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="14.3176470588235"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="10.7725490196078"/>
+    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="8.09803921568627"/>
     <col collapsed="false" hidden="false" max="45" min="45" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="11.6196078431373"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="11.6274509803922"/>
     <col collapsed="false" hidden="false" max="47" min="47" style="0" width="5.52549019607843"/>
     <col collapsed="false" hidden="false" max="48" min="48" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="49" min="49" style="0" width="14.8039215686275"/>
-    <col collapsed="false" hidden="false" max="50" min="50" style="0" width="10.7686274509804"/>
-    <col collapsed="false" hidden="false" max="51" min="51" style="0" width="8.09019607843137"/>
+    <col collapsed="false" hidden="false" max="49" min="49" style="0" width="14.8156862745098"/>
+    <col collapsed="false" hidden="false" max="50" min="50" style="0" width="10.7725490196078"/>
+    <col collapsed="false" hidden="false" max="51" min="51" style="0" width="8.09803921568627"/>
     <col collapsed="false" hidden="false" max="52" min="52" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="53" min="53" style="0" width="11.6196078431373"/>
+    <col collapsed="false" hidden="false" max="53" min="53" style="0" width="11.6274509803922"/>
     <col collapsed="false" hidden="false" max="54" min="54" style="0" width="5.52549019607843"/>
     <col collapsed="false" hidden="false" max="55" min="55" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="56" min="56" style="0" width="15.1490196078431"/>
-    <col collapsed="false" hidden="false" max="57" min="57" style="0" width="10.7686274509804"/>
-    <col collapsed="false" hidden="false" max="58" min="58" style="0" width="8.09019607843137"/>
+    <col collapsed="false" hidden="false" max="56" min="56" style="0" width="15.156862745098"/>
+    <col collapsed="false" hidden="false" max="57" min="57" style="0" width="10.7725490196078"/>
+    <col collapsed="false" hidden="false" max="58" min="58" style="0" width="8.09803921568627"/>
     <col collapsed="false" hidden="false" max="59" min="59" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="60" min="60" style="0" width="11.6196078431373"/>
+    <col collapsed="false" hidden="false" max="60" min="60" style="0" width="11.6274509803922"/>
     <col collapsed="false" hidden="false" max="61" min="61" style="0" width="5.52549019607843"/>
     <col collapsed="false" hidden="false" max="62" min="62" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="63" min="63" style="0" width="10.2705882352941"/>
-    <col collapsed="false" hidden="false" max="64" min="64" style="0" width="8.09019607843137"/>
+    <col collapsed="false" hidden="false" max="63" min="63" style="0" width="10.2745098039216"/>
+    <col collapsed="false" hidden="false" max="64" min="64" style="0" width="8.09803921568627"/>
     <col collapsed="false" hidden="false" max="65" min="65" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="66" min="66" style="0" width="11.6196078431373"/>
+    <col collapsed="false" hidden="false" max="66" min="66" style="0" width="11.6274509803922"/>
     <col collapsed="false" hidden="false" max="67" min="67" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="68" min="68" style="0" width="13.9647058823529"/>
-    <col collapsed="false" hidden="false" max="69" min="69" style="0" width="8.09019607843137"/>
+    <col collapsed="false" hidden="false" max="68" min="68" style="0" width="13.9764705882353"/>
+    <col collapsed="false" hidden="false" max="69" min="69" style="0" width="8.09803921568627"/>
     <col collapsed="false" hidden="false" max="70" min="70" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="71" min="71" style="0" width="11.6196078431373"/>
+    <col collapsed="false" hidden="false" max="71" min="71" style="0" width="11.6274509803922"/>
     <col collapsed="false" hidden="false" max="72" min="72" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="73" min="73" style="0" width="12.9529411764706"/>
-    <col collapsed="false" hidden="false" max="74" min="74" style="0" width="8.09019607843137"/>
+    <col collapsed="false" hidden="false" max="73" min="73" style="0" width="12.9607843137255"/>
+    <col collapsed="false" hidden="false" max="74" min="74" style="0" width="8.09803921568627"/>
     <col collapsed="false" hidden="false" max="75" min="75" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="76" min="76" style="0" width="11.6196078431373"/>
+    <col collapsed="false" hidden="false" max="76" min="76" style="0" width="11.6274509803922"/>
     <col collapsed="false" hidden="false" max="77" min="77" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="78" min="78" style="0" width="12.7882352941176"/>
-    <col collapsed="false" hidden="false" max="79" min="79" style="0" width="8.09019607843137"/>
+    <col collapsed="false" hidden="false" max="78" min="78" style="0" width="12.7960784313726"/>
+    <col collapsed="false" hidden="false" max="79" min="79" style="0" width="8.09803921568627"/>
     <col collapsed="false" hidden="false" max="80" min="80" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="81" min="81" style="0" width="11.6196078431373"/>
+    <col collapsed="false" hidden="false" max="81" min="81" style="0" width="11.6274509803922"/>
     <col collapsed="false" hidden="false" max="82" min="82" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="83" min="83" style="0" width="13.643137254902"/>
-    <col collapsed="false" hidden="false" max="84" min="84" style="0" width="8.09019607843137"/>
+    <col collapsed="false" hidden="false" max="83" min="83" style="0" width="13.6549019607843"/>
+    <col collapsed="false" hidden="false" max="84" min="84" style="0" width="8.09803921568627"/>
     <col collapsed="false" hidden="false" max="85" min="85" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="86" min="86" style="0" width="11.6196078431373"/>
+    <col collapsed="false" hidden="false" max="86" min="86" style="0" width="11.6274509803922"/>
     <col collapsed="false" hidden="false" max="87" min="87" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="88" min="88" style="0" width="14.8039215686275"/>
-    <col collapsed="false" hidden="false" max="89" min="89" style="0" width="8.09019607843137"/>
+    <col collapsed="false" hidden="false" max="88" min="88" style="0" width="14.8156862745098"/>
+    <col collapsed="false" hidden="false" max="89" min="89" style="0" width="8.09803921568627"/>
     <col collapsed="false" hidden="false" max="90" min="90" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="91" min="91" style="0" width="11.6196078431373"/>
+    <col collapsed="false" hidden="false" max="91" min="91" style="0" width="11.6274509803922"/>
     <col collapsed="false" hidden="false" max="92" min="92" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="93" min="93" style="0" width="10.2705882352941"/>
-    <col collapsed="false" hidden="false" max="94" min="94" style="0" width="13.8"/>
-    <col collapsed="false" hidden="false" max="95" min="95" style="0" width="14.8039215686275"/>
-    <col collapsed="false" hidden="false" max="96" min="96" style="0" width="17.3372549019608"/>
+    <col collapsed="false" hidden="false" max="93" min="93" style="0" width="10.2745098039216"/>
+    <col collapsed="false" hidden="false" max="94" min="94" style="0" width="13.8039215686275"/>
+    <col collapsed="false" hidden="false" max="95" min="95" style="0" width="14.8156862745098"/>
+    <col collapsed="false" hidden="false" max="96" min="96" style="0" width="17.3490196078431"/>
     <col collapsed="false" hidden="false" max="97" min="97" style="0" width="6.02352941176471"/>
-    <col collapsed="false" hidden="false" max="98" min="98" style="0" width="23.043137254902"/>
-    <col collapsed="false" hidden="false" max="99" min="99" style="0" width="15.9921568627451"/>
-    <col collapsed="false" hidden="false" max="100" min="100" style="0" width="17.1647058823529"/>
-    <col collapsed="false" hidden="false" max="101" min="101" style="0" width="17.3372549019608"/>
+    <col collapsed="false" hidden="false" max="98" min="98" style="0" width="23.0588235294118"/>
+    <col collapsed="false" hidden="false" max="99" min="99" style="0" width="16.0039215686275"/>
+    <col collapsed="false" hidden="false" max="100" min="100" style="0" width="17.1764705882353"/>
+    <col collapsed="false" hidden="false" max="101" min="101" style="0" width="17.3490196078431"/>
     <col collapsed="false" hidden="false" max="102" min="102" style="0" width="6.02352941176471"/>
-    <col collapsed="false" hidden="false" max="103" min="103" style="0" width="22.2117647058824"/>
-    <col collapsed="false" hidden="false" max="104" min="104" style="0" width="15.9921568627451"/>
-    <col collapsed="false" hidden="false" max="105" min="105" style="0" width="17.1647058823529"/>
-    <col collapsed="false" hidden="false" max="106" min="106" style="0" width="17.3372549019608"/>
+    <col collapsed="false" hidden="false" max="103" min="103" style="0" width="22.2235294117647"/>
+    <col collapsed="false" hidden="false" max="104" min="104" style="0" width="16.0039215686275"/>
+    <col collapsed="false" hidden="false" max="105" min="105" style="0" width="17.1764705882353"/>
+    <col collapsed="false" hidden="false" max="106" min="106" style="0" width="17.3490196078431"/>
     <col collapsed="false" hidden="false" max="107" min="107" style="0" width="6.02352941176471"/>
-    <col collapsed="false" hidden="false" max="108" min="108" style="0" width="11.7764705882353"/>
-    <col collapsed="false" hidden="false" max="109" min="109" style="0" width="17.3372549019608"/>
-    <col collapsed="false" hidden="false" max="110" min="110" style="0" width="12.7882352941176"/>
-    <col collapsed="false" hidden="false" max="111" min="111" style="0" width="18.521568627451"/>
-    <col collapsed="false" hidden="false" max="112" min="112" style="0" width="17.3372549019608"/>
-    <col collapsed="false" hidden="false" max="113" min="113" style="0" width="12.7882352941176"/>
-    <col collapsed="false" hidden="false" max="114" min="114" style="0" width="19.5254901960784"/>
-    <col collapsed="false" hidden="false" max="115" min="115" style="0" width="17.3372549019608"/>
-    <col collapsed="false" hidden="false" max="116" min="116" style="0" width="12.7882352941176"/>
-    <col collapsed="false" hidden="false" max="117" min="117" style="0" width="18.6941176470588"/>
-    <col collapsed="false" hidden="false" max="119" min="118" style="0" width="17.3372549019608"/>
-    <col collapsed="false" hidden="false" max="120" min="120" style="0" width="16.4941176470588"/>
-    <col collapsed="false" hidden="false" max="121" min="121" style="0" width="11.7764705882353"/>
-    <col collapsed="false" hidden="false" max="122" min="122" style="0" width="15.6627450980392"/>
-    <col collapsed="false" hidden="false" max="123" min="123" style="0" width="16.3254901960784"/>
-    <col collapsed="false" hidden="false" max="124" min="124" style="0" width="18.521568627451"/>
-    <col collapsed="false" hidden="false" max="125" min="125" style="0" width="14.4666666666667"/>
-    <col collapsed="false" hidden="false" max="126" min="126" style="0" width="13.643137254902"/>
-    <col collapsed="false" hidden="false" max="138" min="127" style="0" width="18.6941176470588"/>
-    <col collapsed="false" hidden="false" max="140" min="139" style="0" width="30.9725490196078"/>
-    <col collapsed="false" hidden="false" max="141" min="141" style="0" width="26.1019607843137"/>
-    <col collapsed="false" hidden="false" max="142" min="142" style="0" width="20.7098039215686"/>
-    <col collapsed="false" hidden="false" max="143" min="143" style="0" width="13.121568627451"/>
+    <col collapsed="false" hidden="false" max="108" min="108" style="0" width="11.7843137254902"/>
+    <col collapsed="false" hidden="false" max="109" min="109" style="0" width="17.3490196078431"/>
+    <col collapsed="false" hidden="false" max="110" min="110" style="0" width="12.7960784313726"/>
+    <col collapsed="false" hidden="false" max="111" min="111" style="0" width="18.5294117647059"/>
+    <col collapsed="false" hidden="false" max="112" min="112" style="0" width="17.3490196078431"/>
+    <col collapsed="false" hidden="false" max="113" min="113" style="0" width="12.7960784313726"/>
+    <col collapsed="false" hidden="false" max="114" min="114" style="0" width="19.5411764705882"/>
+    <col collapsed="false" hidden="false" max="115" min="115" style="0" width="17.3490196078431"/>
+    <col collapsed="false" hidden="false" max="116" min="116" style="0" width="12.7960784313726"/>
+    <col collapsed="false" hidden="false" max="117" min="117" style="0" width="18.7058823529412"/>
+    <col collapsed="false" hidden="false" max="119" min="118" style="0" width="17.3490196078431"/>
+    <col collapsed="false" hidden="false" max="120" min="120" style="0" width="16.5019607843137"/>
+    <col collapsed="false" hidden="false" max="121" min="121" style="0" width="11.7843137254902"/>
+    <col collapsed="false" hidden="false" max="122" min="122" style="0" width="15.6705882352941"/>
+    <col collapsed="false" hidden="false" max="123" min="123" style="0" width="16.3372549019608"/>
+    <col collapsed="false" hidden="false" max="124" min="124" style="0" width="18.5294117647059"/>
+    <col collapsed="false" hidden="false" max="125" min="125" style="0" width="14.4745098039216"/>
+    <col collapsed="false" hidden="false" max="126" min="126" style="0" width="13.6549019607843"/>
+    <col collapsed="false" hidden="false" max="138" min="127" style="0" width="18.7058823529412"/>
+    <col collapsed="false" hidden="false" max="140" min="139" style="0" width="30.9960784313725"/>
+    <col collapsed="false" hidden="false" max="141" min="141" style="0" width="26.1137254901961"/>
+    <col collapsed="false" hidden="false" max="142" min="142" style="0" width="20.721568627451"/>
+    <col collapsed="false" hidden="false" max="143" min="143" style="0" width="13.1294117647059"/>
     <col collapsed="false" hidden="false" max="144" min="144" style="0" width="7.74117647058824"/>
-    <col collapsed="false" hidden="false" max="145" min="145" style="0" width="13.4588235294118"/>
-    <col collapsed="false" hidden="false" max="146" min="146" style="0" width="10.4313725490196"/>
-    <col collapsed="false" hidden="false" max="1025" min="147" style="0" width="18.6941176470588"/>
+    <col collapsed="false" hidden="false" max="145" min="145" style="0" width="13.4627450980392"/>
+    <col collapsed="false" hidden="false" max="146" min="146" style="0" width="10.4392156862745"/>
+    <col collapsed="false" hidden="false" max="1025" min="147" style="0" width="18.7058823529412"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="1">
@@ -12389,140 +12389,140 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.1058823529412"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.2705882352941"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.92941176470588"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.0196078431373"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.9333333333333"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.478431372549"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.4039215686274"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.4549019607843"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.6627450980392"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="18.6941176470588"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="15.321568627451"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.6117647058824"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="11.9490196078431"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="13.8"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="12.9529411764706"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.9647058823529"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="16.4941176470588"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.278431372549"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="16.3254901960784"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="13.9647058823529"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="10.2705882352941"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="10.7686274509804"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="8.09019607843137"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.1176470588235"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.2745098039216"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.93333333333333"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.0313725490196"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.9490196078431"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.4901960784314"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.4196078431373"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.4588235294118"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.6705882352941"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="18.7058823529412"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="15.3333333333333"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.6235294117647"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="11.956862745098"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="13.8039215686275"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="12.9607843137255"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.9764705882353"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="16.5019607843137"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.2901960784314"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="16.3372549019608"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="13.9764705882353"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="10.2745098039216"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="10.7725490196078"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="8.09803921568627"/>
     <col collapsed="false" hidden="false" max="24" min="24" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="11.6196078431373"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="11.6274509803922"/>
     <col collapsed="false" hidden="false" max="26" min="26" style="0" width="5.52549019607843"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="11.6196078431373"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="14.1333333333333"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="10.7686274509804"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="8.09019607843137"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="11.6274509803922"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="14.1411764705882"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="10.7725490196078"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="8.09803921568627"/>
     <col collapsed="false" hidden="false" max="31" min="31" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="11.6196078431373"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="11.6274509803922"/>
     <col collapsed="false" hidden="false" max="33" min="33" style="0" width="5.52549019607843"/>
     <col collapsed="false" hidden="false" max="34" min="34" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="14.6509803921569"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="10.7686274509804"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="8.09019607843137"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="14.6588235294118"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="10.7725490196078"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="8.09803921568627"/>
     <col collapsed="false" hidden="false" max="38" min="38" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="11.6196078431373"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="11.6274509803922"/>
     <col collapsed="false" hidden="false" max="40" min="40" style="0" width="5.52549019607843"/>
     <col collapsed="false" hidden="false" max="41" min="41" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="14.3058823529412"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="10.7686274509804"/>
-    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="8.09019607843137"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="14.3176470588235"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="10.7725490196078"/>
+    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="8.09803921568627"/>
     <col collapsed="false" hidden="false" max="45" min="45" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="11.6196078431373"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="11.6274509803922"/>
     <col collapsed="false" hidden="false" max="47" min="47" style="0" width="5.52549019607843"/>
     <col collapsed="false" hidden="false" max="48" min="48" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="49" min="49" style="0" width="14.8039215686275"/>
-    <col collapsed="false" hidden="false" max="50" min="50" style="0" width="10.7686274509804"/>
-    <col collapsed="false" hidden="false" max="51" min="51" style="0" width="8.09019607843137"/>
+    <col collapsed="false" hidden="false" max="49" min="49" style="0" width="14.8156862745098"/>
+    <col collapsed="false" hidden="false" max="50" min="50" style="0" width="10.7725490196078"/>
+    <col collapsed="false" hidden="false" max="51" min="51" style="0" width="8.09803921568627"/>
     <col collapsed="false" hidden="false" max="52" min="52" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="53" min="53" style="0" width="11.6196078431373"/>
+    <col collapsed="false" hidden="false" max="53" min="53" style="0" width="11.6274509803922"/>
     <col collapsed="false" hidden="false" max="54" min="54" style="0" width="5.52549019607843"/>
     <col collapsed="false" hidden="false" max="55" min="55" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="56" min="56" style="0" width="15.1490196078431"/>
-    <col collapsed="false" hidden="false" max="57" min="57" style="0" width="10.7686274509804"/>
-    <col collapsed="false" hidden="false" max="58" min="58" style="0" width="8.09019607843137"/>
+    <col collapsed="false" hidden="false" max="56" min="56" style="0" width="15.156862745098"/>
+    <col collapsed="false" hidden="false" max="57" min="57" style="0" width="10.7725490196078"/>
+    <col collapsed="false" hidden="false" max="58" min="58" style="0" width="8.09803921568627"/>
     <col collapsed="false" hidden="false" max="59" min="59" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="60" min="60" style="0" width="11.6196078431373"/>
+    <col collapsed="false" hidden="false" max="60" min="60" style="0" width="11.6274509803922"/>
     <col collapsed="false" hidden="false" max="61" min="61" style="0" width="5.52549019607843"/>
     <col collapsed="false" hidden="false" max="62" min="62" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="63" min="63" style="0" width="10.2705882352941"/>
-    <col collapsed="false" hidden="false" max="64" min="64" style="0" width="8.09019607843137"/>
+    <col collapsed="false" hidden="false" max="63" min="63" style="0" width="10.2745098039216"/>
+    <col collapsed="false" hidden="false" max="64" min="64" style="0" width="8.09803921568627"/>
     <col collapsed="false" hidden="false" max="65" min="65" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="66" min="66" style="0" width="11.6196078431373"/>
+    <col collapsed="false" hidden="false" max="66" min="66" style="0" width="11.6274509803922"/>
     <col collapsed="false" hidden="false" max="67" min="67" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="68" min="68" style="0" width="13.9647058823529"/>
-    <col collapsed="false" hidden="false" max="69" min="69" style="0" width="8.09019607843137"/>
+    <col collapsed="false" hidden="false" max="68" min="68" style="0" width="13.9764705882353"/>
+    <col collapsed="false" hidden="false" max="69" min="69" style="0" width="8.09803921568627"/>
     <col collapsed="false" hidden="false" max="70" min="70" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="71" min="71" style="0" width="11.6196078431373"/>
+    <col collapsed="false" hidden="false" max="71" min="71" style="0" width="11.6274509803922"/>
     <col collapsed="false" hidden="false" max="72" min="72" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="73" min="73" style="0" width="12.9529411764706"/>
-    <col collapsed="false" hidden="false" max="74" min="74" style="0" width="8.09019607843137"/>
+    <col collapsed="false" hidden="false" max="73" min="73" style="0" width="12.9607843137255"/>
+    <col collapsed="false" hidden="false" max="74" min="74" style="0" width="8.09803921568627"/>
     <col collapsed="false" hidden="false" max="75" min="75" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="76" min="76" style="0" width="11.6196078431373"/>
+    <col collapsed="false" hidden="false" max="76" min="76" style="0" width="11.6274509803922"/>
     <col collapsed="false" hidden="false" max="77" min="77" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="78" min="78" style="0" width="12.7882352941176"/>
-    <col collapsed="false" hidden="false" max="79" min="79" style="0" width="8.09019607843137"/>
+    <col collapsed="false" hidden="false" max="78" min="78" style="0" width="12.7960784313726"/>
+    <col collapsed="false" hidden="false" max="79" min="79" style="0" width="8.09803921568627"/>
     <col collapsed="false" hidden="false" max="80" min="80" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="81" min="81" style="0" width="11.6196078431373"/>
+    <col collapsed="false" hidden="false" max="81" min="81" style="0" width="11.6274509803922"/>
     <col collapsed="false" hidden="false" max="82" min="82" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="83" min="83" style="0" width="13.643137254902"/>
-    <col collapsed="false" hidden="false" max="84" min="84" style="0" width="8.09019607843137"/>
+    <col collapsed="false" hidden="false" max="83" min="83" style="0" width="13.6549019607843"/>
+    <col collapsed="false" hidden="false" max="84" min="84" style="0" width="8.09803921568627"/>
     <col collapsed="false" hidden="false" max="85" min="85" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="86" min="86" style="0" width="11.6196078431373"/>
+    <col collapsed="false" hidden="false" max="86" min="86" style="0" width="11.6274509803922"/>
     <col collapsed="false" hidden="false" max="87" min="87" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="88" min="88" style="0" width="14.8039215686275"/>
-    <col collapsed="false" hidden="false" max="89" min="89" style="0" width="8.09019607843137"/>
+    <col collapsed="false" hidden="false" max="88" min="88" style="0" width="14.8156862745098"/>
+    <col collapsed="false" hidden="false" max="89" min="89" style="0" width="8.09803921568627"/>
     <col collapsed="false" hidden="false" max="90" min="90" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="91" min="91" style="0" width="11.6196078431373"/>
+    <col collapsed="false" hidden="false" max="91" min="91" style="0" width="11.6274509803922"/>
     <col collapsed="false" hidden="false" max="92" min="92" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="93" min="93" style="0" width="10.2705882352941"/>
-    <col collapsed="false" hidden="false" max="94" min="94" style="0" width="13.8"/>
-    <col collapsed="false" hidden="false" max="95" min="95" style="0" width="14.8039215686275"/>
-    <col collapsed="false" hidden="false" max="96" min="96" style="0" width="17.3372549019608"/>
+    <col collapsed="false" hidden="false" max="93" min="93" style="0" width="10.2745098039216"/>
+    <col collapsed="false" hidden="false" max="94" min="94" style="0" width="13.8039215686275"/>
+    <col collapsed="false" hidden="false" max="95" min="95" style="0" width="14.8156862745098"/>
+    <col collapsed="false" hidden="false" max="96" min="96" style="0" width="17.3490196078431"/>
     <col collapsed="false" hidden="false" max="97" min="97" style="0" width="6.02352941176471"/>
-    <col collapsed="false" hidden="false" max="98" min="98" style="0" width="23.043137254902"/>
-    <col collapsed="false" hidden="false" max="99" min="99" style="0" width="15.9921568627451"/>
-    <col collapsed="false" hidden="false" max="100" min="100" style="0" width="17.1647058823529"/>
-    <col collapsed="false" hidden="false" max="101" min="101" style="0" width="17.3372549019608"/>
+    <col collapsed="false" hidden="false" max="98" min="98" style="0" width="23.0588235294118"/>
+    <col collapsed="false" hidden="false" max="99" min="99" style="0" width="16.0039215686275"/>
+    <col collapsed="false" hidden="false" max="100" min="100" style="0" width="17.1764705882353"/>
+    <col collapsed="false" hidden="false" max="101" min="101" style="0" width="17.3490196078431"/>
     <col collapsed="false" hidden="false" max="102" min="102" style="0" width="6.02352941176471"/>
-    <col collapsed="false" hidden="false" max="103" min="103" style="0" width="22.2117647058824"/>
-    <col collapsed="false" hidden="false" max="104" min="104" style="0" width="15.9921568627451"/>
-    <col collapsed="false" hidden="false" max="105" min="105" style="0" width="17.1647058823529"/>
-    <col collapsed="false" hidden="false" max="106" min="106" style="0" width="17.3372549019608"/>
+    <col collapsed="false" hidden="false" max="103" min="103" style="0" width="22.2235294117647"/>
+    <col collapsed="false" hidden="false" max="104" min="104" style="0" width="16.0039215686275"/>
+    <col collapsed="false" hidden="false" max="105" min="105" style="0" width="17.1764705882353"/>
+    <col collapsed="false" hidden="false" max="106" min="106" style="0" width="17.3490196078431"/>
     <col collapsed="false" hidden="false" max="107" min="107" style="0" width="6.02352941176471"/>
-    <col collapsed="false" hidden="false" max="108" min="108" style="0" width="11.7764705882353"/>
-    <col collapsed="false" hidden="false" max="109" min="109" style="0" width="17.3372549019608"/>
-    <col collapsed="false" hidden="false" max="110" min="110" style="0" width="12.7882352941176"/>
-    <col collapsed="false" hidden="false" max="111" min="111" style="0" width="18.521568627451"/>
-    <col collapsed="false" hidden="false" max="112" min="112" style="0" width="17.3372549019608"/>
-    <col collapsed="false" hidden="false" max="113" min="113" style="0" width="12.7882352941176"/>
-    <col collapsed="false" hidden="false" max="114" min="114" style="0" width="19.5254901960784"/>
-    <col collapsed="false" hidden="false" max="115" min="115" style="0" width="17.3372549019608"/>
-    <col collapsed="false" hidden="false" max="116" min="116" style="0" width="12.7882352941176"/>
-    <col collapsed="false" hidden="false" max="117" min="117" style="0" width="18.6941176470588"/>
-    <col collapsed="false" hidden="false" max="119" min="118" style="0" width="17.3372549019608"/>
-    <col collapsed="false" hidden="false" max="120" min="120" style="0" width="16.4941176470588"/>
-    <col collapsed="false" hidden="false" max="121" min="121" style="0" width="11.7764705882353"/>
-    <col collapsed="false" hidden="false" max="122" min="122" style="0" width="15.6627450980392"/>
-    <col collapsed="false" hidden="false" max="123" min="123" style="0" width="16.3254901960784"/>
-    <col collapsed="false" hidden="false" max="124" min="124" style="0" width="18.521568627451"/>
-    <col collapsed="false" hidden="false" max="125" min="125" style="0" width="14.4666666666667"/>
-    <col collapsed="false" hidden="false" max="126" min="126" style="0" width="13.643137254902"/>
-    <col collapsed="false" hidden="false" max="138" min="127" style="0" width="18.6941176470588"/>
-    <col collapsed="false" hidden="false" max="140" min="139" style="0" width="30.9725490196078"/>
-    <col collapsed="false" hidden="false" max="141" min="141" style="0" width="26.1019607843137"/>
-    <col collapsed="false" hidden="false" max="142" min="142" style="0" width="20.7098039215686"/>
-    <col collapsed="false" hidden="false" max="143" min="143" style="0" width="13.121568627451"/>
+    <col collapsed="false" hidden="false" max="108" min="108" style="0" width="11.7843137254902"/>
+    <col collapsed="false" hidden="false" max="109" min="109" style="0" width="17.3490196078431"/>
+    <col collapsed="false" hidden="false" max="110" min="110" style="0" width="12.7960784313726"/>
+    <col collapsed="false" hidden="false" max="111" min="111" style="0" width="18.5294117647059"/>
+    <col collapsed="false" hidden="false" max="112" min="112" style="0" width="17.3490196078431"/>
+    <col collapsed="false" hidden="false" max="113" min="113" style="0" width="12.7960784313726"/>
+    <col collapsed="false" hidden="false" max="114" min="114" style="0" width="19.5411764705882"/>
+    <col collapsed="false" hidden="false" max="115" min="115" style="0" width="17.3490196078431"/>
+    <col collapsed="false" hidden="false" max="116" min="116" style="0" width="12.7960784313726"/>
+    <col collapsed="false" hidden="false" max="117" min="117" style="0" width="18.7058823529412"/>
+    <col collapsed="false" hidden="false" max="119" min="118" style="0" width="17.3490196078431"/>
+    <col collapsed="false" hidden="false" max="120" min="120" style="0" width="16.5019607843137"/>
+    <col collapsed="false" hidden="false" max="121" min="121" style="0" width="11.7843137254902"/>
+    <col collapsed="false" hidden="false" max="122" min="122" style="0" width="15.6705882352941"/>
+    <col collapsed="false" hidden="false" max="123" min="123" style="0" width="16.3372549019608"/>
+    <col collapsed="false" hidden="false" max="124" min="124" style="0" width="18.5294117647059"/>
+    <col collapsed="false" hidden="false" max="125" min="125" style="0" width="14.4745098039216"/>
+    <col collapsed="false" hidden="false" max="126" min="126" style="0" width="13.6549019607843"/>
+    <col collapsed="false" hidden="false" max="138" min="127" style="0" width="18.7058823529412"/>
+    <col collapsed="false" hidden="false" max="140" min="139" style="0" width="30.9960784313725"/>
+    <col collapsed="false" hidden="false" max="141" min="141" style="0" width="26.1137254901961"/>
+    <col collapsed="false" hidden="false" max="142" min="142" style="0" width="20.721568627451"/>
+    <col collapsed="false" hidden="false" max="143" min="143" style="0" width="13.1294117647059"/>
     <col collapsed="false" hidden="false" max="144" min="144" style="0" width="7.74117647058824"/>
-    <col collapsed="false" hidden="false" max="145" min="145" style="0" width="13.4588235294118"/>
-    <col collapsed="false" hidden="false" max="146" min="146" style="0" width="10.4313725490196"/>
-    <col collapsed="false" hidden="false" max="1025" min="147" style="0" width="18.6941176470588"/>
+    <col collapsed="false" hidden="false" max="145" min="145" style="0" width="13.4627450980392"/>
+    <col collapsed="false" hidden="false" max="146" min="146" style="0" width="10.4392156862745"/>
+    <col collapsed="false" hidden="false" max="1025" min="147" style="0" width="18.7058823529412"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="1">

</xml_diff>

<commit_message>
more executive top5 validations
</commit_message>
<xml_diff>
--- a/core/test/input/FullValuesOnly.xlsx
+++ b/core/test/input/FullValuesOnly.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="3" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="245" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="4" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="245" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="DOC_SRC" sheetId="1" state="visible" r:id="rId2"/>
@@ -1168,17 +1168,17 @@
   </sheetPr>
   <dimension ref="A1:T68"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A31" view="normal" windowProtection="false" workbookViewId="0" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A16" view="normal" windowProtection="false" workbookViewId="0" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100">
       <selection activeCell="B42" activeCellId="0" pane="topLeft" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.6627450980392"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.9176470588235"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.0627450980392"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.2392156862745"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.5450980392157"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.7686274509804"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7137254901961"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.0235294117647"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.1764705882353"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.356862745098"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.6313725490196"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.8078431372549"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="1">
@@ -2644,145 +2644,145 @@
   </sheetPr>
   <dimension ref="A1:EP32"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="DS1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100">
-      <selection activeCell="DV4" activeCellId="0" pane="topLeft" sqref="DV4"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="BE1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100">
+      <selection activeCell="BL22" activeCellId="0" pane="topLeft" sqref="BL22"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.1176470588235"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.2745098039216"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.93333333333333"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.0313725490196"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.9490196078431"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.4901960784314"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.4196078431373"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.4588235294118"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.6705882352941"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="18.7058823529412"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="15.3333333333333"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.6235294117647"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="11.956862745098"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="13.8039215686275"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="12.9607843137255"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.9764705882353"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="16.5019607843137"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.2901960784314"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="16.3372549019608"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="13.9764705882353"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="10.2745098039216"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="10.7725490196078"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="8.09803921568627"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.2313725490196"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.3137254901961"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.98039215686275"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.1098039215686"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.0666666666667"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.5372549019608"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.5176470588235"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.5058823529412"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.7411764705882"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="18.7803921568627"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="15.4"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.6627450980392"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="12"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="13.8509803921569"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="13.0117647058824"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="14.0274509803922"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="16.5686274509804"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.3294117647059"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="16.4039215686274"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="14.0274509803922"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="10.3137254901961"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="10.8117647058824"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="8.10196078431373"/>
     <col collapsed="false" hidden="false" max="24" min="24" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="11.6274509803922"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="11.6666666666667"/>
     <col collapsed="false" hidden="false" max="26" min="26" style="0" width="5.52549019607843"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="11.6274509803922"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="14.1411764705882"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="10.7725490196078"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="8.09803921568627"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="11.6666666666667"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="14.1921568627451"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="10.8117647058824"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="8.10196078431373"/>
     <col collapsed="false" hidden="false" max="31" min="31" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="11.6274509803922"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="11.6666666666667"/>
     <col collapsed="false" hidden="false" max="33" min="33" style="0" width="5.52549019607843"/>
     <col collapsed="false" hidden="false" max="34" min="34" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="14.6588235294118"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="10.7725490196078"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="8.09803921568627"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="14.7176470588235"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="10.8117647058824"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="8.10196078431373"/>
     <col collapsed="false" hidden="false" max="38" min="38" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="11.6274509803922"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="11.6666666666667"/>
     <col collapsed="false" hidden="false" max="40" min="40" style="0" width="5.52549019607843"/>
     <col collapsed="false" hidden="false" max="41" min="41" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="14.3176470588235"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="10.7725490196078"/>
-    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="8.09803921568627"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="14.3764705882353"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="10.8117647058824"/>
+    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="8.10196078431373"/>
     <col collapsed="false" hidden="false" max="45" min="45" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="11.6274509803922"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="11.6666666666667"/>
     <col collapsed="false" hidden="false" max="47" min="47" style="0" width="5.52549019607843"/>
     <col collapsed="false" hidden="false" max="48" min="48" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="49" min="49" style="0" width="14.8156862745098"/>
-    <col collapsed="false" hidden="false" max="50" min="50" style="0" width="10.7725490196078"/>
-    <col collapsed="false" hidden="false" max="51" min="51" style="0" width="8.09803921568627"/>
+    <col collapsed="false" hidden="false" max="49" min="49" style="0" width="14.8745098039216"/>
+    <col collapsed="false" hidden="false" max="50" min="50" style="0" width="10.8117647058824"/>
+    <col collapsed="false" hidden="false" max="51" min="51" style="0" width="8.10196078431373"/>
     <col collapsed="false" hidden="false" max="52" min="52" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="53" min="53" style="0" width="11.6274509803922"/>
+    <col collapsed="false" hidden="false" max="53" min="53" style="0" width="11.6666666666667"/>
     <col collapsed="false" hidden="false" max="54" min="54" style="0" width="5.52549019607843"/>
     <col collapsed="false" hidden="false" max="55" min="55" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="56" min="56" style="0" width="15.156862745098"/>
-    <col collapsed="false" hidden="false" max="57" min="57" style="0" width="10.7725490196078"/>
-    <col collapsed="false" hidden="false" max="58" min="58" style="0" width="8.09803921568627"/>
+    <col collapsed="false" hidden="false" max="56" min="56" style="0" width="15.2156862745098"/>
+    <col collapsed="false" hidden="false" max="57" min="57" style="0" width="10.8117647058824"/>
+    <col collapsed="false" hidden="false" max="58" min="58" style="0" width="8.10196078431373"/>
     <col collapsed="false" hidden="false" max="59" min="59" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="60" min="60" style="0" width="11.6274509803922"/>
+    <col collapsed="false" hidden="false" max="60" min="60" style="0" width="11.6666666666667"/>
     <col collapsed="false" hidden="false" max="61" min="61" style="0" width="5.52549019607843"/>
     <col collapsed="false" hidden="false" max="62" min="62" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="63" min="63" style="0" width="10.2745098039216"/>
-    <col collapsed="false" hidden="false" max="64" min="64" style="0" width="8.09803921568627"/>
+    <col collapsed="false" hidden="false" max="63" min="63" style="0" width="10.3137254901961"/>
+    <col collapsed="false" hidden="false" max="64" min="64" style="0" width="8.10196078431373"/>
     <col collapsed="false" hidden="false" max="65" min="65" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="66" min="66" style="0" width="11.6274509803922"/>
+    <col collapsed="false" hidden="false" max="66" min="66" style="0" width="11.6666666666667"/>
     <col collapsed="false" hidden="false" max="67" min="67" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="68" min="68" style="0" width="13.9764705882353"/>
-    <col collapsed="false" hidden="false" max="69" min="69" style="0" width="8.09803921568627"/>
+    <col collapsed="false" hidden="false" max="68" min="68" style="0" width="14.0274509803922"/>
+    <col collapsed="false" hidden="false" max="69" min="69" style="0" width="8.10196078431373"/>
     <col collapsed="false" hidden="false" max="70" min="70" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="71" min="71" style="0" width="11.6274509803922"/>
+    <col collapsed="false" hidden="false" max="71" min="71" style="0" width="11.6666666666667"/>
     <col collapsed="false" hidden="false" max="72" min="72" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="73" min="73" style="0" width="12.9607843137255"/>
-    <col collapsed="false" hidden="false" max="74" min="74" style="0" width="8.09803921568627"/>
+    <col collapsed="false" hidden="false" max="73" min="73" style="0" width="13.0117647058824"/>
+    <col collapsed="false" hidden="false" max="74" min="74" style="0" width="8.10196078431373"/>
     <col collapsed="false" hidden="false" max="75" min="75" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="76" min="76" style="0" width="11.6274509803922"/>
+    <col collapsed="false" hidden="false" max="76" min="76" style="0" width="11.6666666666667"/>
     <col collapsed="false" hidden="false" max="77" min="77" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="78" min="78" style="0" width="12.7960784313726"/>
-    <col collapsed="false" hidden="false" max="79" min="79" style="0" width="8.09803921568627"/>
+    <col collapsed="false" hidden="false" max="78" min="78" style="0" width="12.8352941176471"/>
+    <col collapsed="false" hidden="false" max="79" min="79" style="0" width="8.10196078431373"/>
     <col collapsed="false" hidden="false" max="80" min="80" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="81" min="81" style="0" width="11.6274509803922"/>
+    <col collapsed="false" hidden="false" max="81" min="81" style="0" width="11.6666666666667"/>
     <col collapsed="false" hidden="false" max="82" min="82" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="83" min="83" style="0" width="13.6549019607843"/>
-    <col collapsed="false" hidden="false" max="84" min="84" style="0" width="8.09803921568627"/>
+    <col collapsed="false" hidden="false" max="83" min="83" style="0" width="13.7058823529412"/>
+    <col collapsed="false" hidden="false" max="84" min="84" style="0" width="8.10196078431373"/>
     <col collapsed="false" hidden="false" max="85" min="85" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="86" min="86" style="0" width="11.6274509803922"/>
+    <col collapsed="false" hidden="false" max="86" min="86" style="0" width="11.6666666666667"/>
     <col collapsed="false" hidden="false" max="87" min="87" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="88" min="88" style="0" width="14.8156862745098"/>
-    <col collapsed="false" hidden="false" max="89" min="89" style="0" width="8.09803921568627"/>
+    <col collapsed="false" hidden="false" max="88" min="88" style="0" width="14.8745098039216"/>
+    <col collapsed="false" hidden="false" max="89" min="89" style="0" width="8.10196078431373"/>
     <col collapsed="false" hidden="false" max="90" min="90" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="91" min="91" style="0" width="11.6274509803922"/>
+    <col collapsed="false" hidden="false" max="91" min="91" style="0" width="11.6666666666667"/>
     <col collapsed="false" hidden="false" max="92" min="92" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="93" min="93" style="0" width="10.2745098039216"/>
-    <col collapsed="false" hidden="false" max="94" min="94" style="0" width="13.8039215686275"/>
-    <col collapsed="false" hidden="false" max="95" min="95" style="0" width="14.8156862745098"/>
-    <col collapsed="false" hidden="false" max="96" min="96" style="0" width="17.3490196078431"/>
+    <col collapsed="false" hidden="false" max="93" min="93" style="0" width="10.3137254901961"/>
+    <col collapsed="false" hidden="false" max="94" min="94" style="0" width="13.8509803921569"/>
+    <col collapsed="false" hidden="false" max="95" min="95" style="0" width="14.8745098039216"/>
+    <col collapsed="false" hidden="false" max="96" min="96" style="0" width="17.4274509803922"/>
     <col collapsed="false" hidden="false" max="97" min="97" style="0" width="6.02352941176471"/>
-    <col collapsed="false" hidden="false" max="98" min="98" style="0" width="23.0588235294118"/>
-    <col collapsed="false" hidden="false" max="99" min="99" style="0" width="16.0039215686275"/>
-    <col collapsed="false" hidden="false" max="100" min="100" style="0" width="17.1764705882353"/>
-    <col collapsed="false" hidden="false" max="101" min="101" style="0" width="17.3490196078431"/>
+    <col collapsed="false" hidden="false" max="98" min="98" style="0" width="23.156862745098"/>
+    <col collapsed="false" hidden="false" max="99" min="99" style="0" width="16.0705882352941"/>
+    <col collapsed="false" hidden="false" max="100" min="100" style="0" width="17.2509803921569"/>
+    <col collapsed="false" hidden="false" max="101" min="101" style="0" width="17.4274509803922"/>
     <col collapsed="false" hidden="false" max="102" min="102" style="0" width="6.02352941176471"/>
-    <col collapsed="false" hidden="false" max="103" min="103" style="0" width="22.2235294117647"/>
-    <col collapsed="false" hidden="false" max="104" min="104" style="0" width="16.0039215686275"/>
-    <col collapsed="false" hidden="false" max="105" min="105" style="0" width="17.1764705882353"/>
-    <col collapsed="false" hidden="false" max="106" min="106" style="0" width="17.3490196078431"/>
+    <col collapsed="false" hidden="false" max="103" min="103" style="0" width="22.3098039215686"/>
+    <col collapsed="false" hidden="false" max="104" min="104" style="0" width="16.0705882352941"/>
+    <col collapsed="false" hidden="false" max="105" min="105" style="0" width="17.2509803921569"/>
+    <col collapsed="false" hidden="false" max="106" min="106" style="0" width="17.4274509803922"/>
     <col collapsed="false" hidden="false" max="107" min="107" style="0" width="6.02352941176471"/>
-    <col collapsed="false" hidden="false" max="108" min="108" style="0" width="11.7843137254902"/>
-    <col collapsed="false" hidden="false" max="109" min="109" style="0" width="17.3490196078431"/>
-    <col collapsed="false" hidden="false" max="110" min="110" style="0" width="12.7960784313726"/>
-    <col collapsed="false" hidden="false" max="111" min="111" style="0" width="18.5294117647059"/>
-    <col collapsed="false" hidden="false" max="112" min="112" style="0" width="17.3490196078431"/>
-    <col collapsed="false" hidden="false" max="113" min="113" style="0" width="12.7960784313726"/>
-    <col collapsed="false" hidden="false" max="114" min="114" style="0" width="19.5411764705882"/>
-    <col collapsed="false" hidden="false" max="115" min="115" style="0" width="17.3490196078431"/>
-    <col collapsed="false" hidden="false" max="116" min="116" style="0" width="12.7960784313726"/>
-    <col collapsed="false" hidden="false" max="117" min="117" style="0" width="18.7058823529412"/>
-    <col collapsed="false" hidden="false" max="119" min="118" style="0" width="17.3490196078431"/>
-    <col collapsed="false" hidden="false" max="120" min="120" style="0" width="16.5019607843137"/>
-    <col collapsed="false" hidden="false" max="121" min="121" style="0" width="11.7843137254902"/>
-    <col collapsed="false" hidden="false" max="122" min="122" style="0" width="15.6705882352941"/>
-    <col collapsed="false" hidden="false" max="123" min="123" style="0" width="16.3372549019608"/>
-    <col collapsed="false" hidden="false" max="124" min="124" style="0" width="18.5294117647059"/>
-    <col collapsed="false" hidden="false" max="125" min="125" style="0" width="14.4745098039216"/>
-    <col collapsed="false" hidden="false" max="126" min="126" style="0" width="13.6549019607843"/>
-    <col collapsed="false" hidden="false" max="138" min="127" style="0" width="18.7058823529412"/>
-    <col collapsed="false" hidden="false" max="140" min="139" style="0" width="30.9960784313725"/>
-    <col collapsed="false" hidden="false" max="141" min="141" style="0" width="26.1137254901961"/>
-    <col collapsed="false" hidden="false" max="142" min="142" style="0" width="20.721568627451"/>
-    <col collapsed="false" hidden="false" max="143" min="143" style="0" width="13.1294117647059"/>
+    <col collapsed="false" hidden="false" max="108" min="108" style="0" width="11.8235294117647"/>
+    <col collapsed="false" hidden="false" max="109" min="109" style="0" width="17.4274509803922"/>
+    <col collapsed="false" hidden="false" max="110" min="110" style="0" width="12.8352941176471"/>
+    <col collapsed="false" hidden="false" max="111" min="111" style="0" width="18.6078431372549"/>
+    <col collapsed="false" hidden="false" max="112" min="112" style="0" width="17.4274509803922"/>
+    <col collapsed="false" hidden="false" max="113" min="113" style="0" width="12.8352941176471"/>
+    <col collapsed="false" hidden="false" max="114" min="114" style="0" width="19.6274509803922"/>
+    <col collapsed="false" hidden="false" max="115" min="115" style="0" width="17.4274509803922"/>
+    <col collapsed="false" hidden="false" max="116" min="116" style="0" width="12.8352941176471"/>
+    <col collapsed="false" hidden="false" max="117" min="117" style="0" width="18.7803921568627"/>
+    <col collapsed="false" hidden="false" max="119" min="118" style="0" width="17.4274509803922"/>
+    <col collapsed="false" hidden="false" max="120" min="120" style="0" width="16.5686274509804"/>
+    <col collapsed="false" hidden="false" max="121" min="121" style="0" width="11.8235294117647"/>
+    <col collapsed="false" hidden="false" max="122" min="122" style="0" width="15.7411764705882"/>
+    <col collapsed="false" hidden="false" max="123" min="123" style="0" width="16.4039215686274"/>
+    <col collapsed="false" hidden="false" max="124" min="124" style="0" width="18.6078431372549"/>
+    <col collapsed="false" hidden="false" max="125" min="125" style="0" width="14.5254901960784"/>
+    <col collapsed="false" hidden="false" max="126" min="126" style="0" width="13.7058823529412"/>
+    <col collapsed="false" hidden="false" max="138" min="127" style="0" width="18.7803921568627"/>
+    <col collapsed="false" hidden="false" max="140" min="139" style="0" width="31.1137254901961"/>
+    <col collapsed="false" hidden="false" max="141" min="141" style="0" width="26.2274509803922"/>
+    <col collapsed="false" hidden="false" max="142" min="142" style="0" width="20.8"/>
+    <col collapsed="false" hidden="false" max="143" min="143" style="0" width="13.1764705882353"/>
     <col collapsed="false" hidden="false" max="144" min="144" style="0" width="7.74117647058824"/>
-    <col collapsed="false" hidden="false" max="145" min="145" style="0" width="13.4627450980392"/>
-    <col collapsed="false" hidden="false" max="146" min="146" style="0" width="10.4392156862745"/>
-    <col collapsed="false" hidden="false" max="1025" min="147" style="0" width="18.7058823529412"/>
+    <col collapsed="false" hidden="false" max="145" min="145" style="0" width="13.5176470588235"/>
+    <col collapsed="false" hidden="false" max="146" min="146" style="0" width="10.478431372549"/>
+    <col collapsed="false" hidden="false" max="1025" min="147" style="0" width="18.7803921568627"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="1">
@@ -3682,7 +3682,7 @@
         <v>100</v>
       </c>
       <c r="BM4" s="66" t="n">
-        <v>200</v>
+        <v>3</v>
       </c>
       <c r="BN4" s="66" t="n">
         <v>300</v>
@@ -3745,17 +3745,17 @@
       <c r="DN4" s="66"/>
       <c r="DO4" s="66"/>
       <c r="DP4" s="66" t="n">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="DQ4" s="66"/>
       <c r="DR4" s="66"/>
       <c r="DS4" s="66"/>
       <c r="DT4" s="66" t="n">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="DU4" s="66"/>
       <c r="DV4" s="66" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="DW4" s="66"/>
       <c r="DX4" s="66"/>
@@ -7514,145 +7514,145 @@
   </sheetPr>
   <dimension ref="A1:EP32"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="I1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100">
-      <selection activeCell="L4" activeCellId="0" pane="topLeft" sqref="L4"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="DQ1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100">
+      <selection activeCell="DT4" activeCellId="0" pane="topLeft" sqref="DT4"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.1176470588235"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.2745098039216"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.93333333333333"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.0313725490196"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.9490196078431"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.4901960784314"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.4196078431373"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.4588235294118"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.6705882352941"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="18.7058823529412"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="15.3333333333333"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.6235294117647"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="11.956862745098"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="13.8039215686275"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="12.9607843137255"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.9764705882353"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="16.5019607843137"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.2901960784314"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="16.3372549019608"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="13.9764705882353"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="10.2745098039216"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="10.7725490196078"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="8.09803921568627"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.2313725490196"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.3137254901961"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.98039215686275"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.1098039215686"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.0666666666667"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.5372549019608"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.5176470588235"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.5058823529412"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.7411764705882"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="18.7803921568627"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="15.4"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.6627450980392"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="12"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="13.8509803921569"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="13.0117647058824"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="14.0274509803922"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="16.5686274509804"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.3294117647059"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="16.4039215686274"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="14.0274509803922"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="10.3137254901961"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="10.8117647058824"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="8.10196078431373"/>
     <col collapsed="false" hidden="false" max="24" min="24" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="11.6274509803922"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="11.6666666666667"/>
     <col collapsed="false" hidden="false" max="26" min="26" style="0" width="5.52549019607843"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="11.6274509803922"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="14.1411764705882"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="10.7725490196078"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="8.09803921568627"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="11.6666666666667"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="14.1921568627451"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="10.8117647058824"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="8.10196078431373"/>
     <col collapsed="false" hidden="false" max="31" min="31" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="11.6274509803922"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="11.6666666666667"/>
     <col collapsed="false" hidden="false" max="33" min="33" style="0" width="5.52549019607843"/>
     <col collapsed="false" hidden="false" max="34" min="34" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="14.6588235294118"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="10.7725490196078"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="8.09803921568627"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="14.7176470588235"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="10.8117647058824"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="8.10196078431373"/>
     <col collapsed="false" hidden="false" max="38" min="38" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="11.6274509803922"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="11.6666666666667"/>
     <col collapsed="false" hidden="false" max="40" min="40" style="0" width="5.52549019607843"/>
     <col collapsed="false" hidden="false" max="41" min="41" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="14.3176470588235"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="10.7725490196078"/>
-    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="8.09803921568627"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="14.3764705882353"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="10.8117647058824"/>
+    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="8.10196078431373"/>
     <col collapsed="false" hidden="false" max="45" min="45" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="11.6274509803922"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="11.6666666666667"/>
     <col collapsed="false" hidden="false" max="47" min="47" style="0" width="5.52549019607843"/>
     <col collapsed="false" hidden="false" max="48" min="48" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="49" min="49" style="0" width="14.8156862745098"/>
-    <col collapsed="false" hidden="false" max="50" min="50" style="0" width="10.7725490196078"/>
-    <col collapsed="false" hidden="false" max="51" min="51" style="0" width="8.09803921568627"/>
+    <col collapsed="false" hidden="false" max="49" min="49" style="0" width="14.8745098039216"/>
+    <col collapsed="false" hidden="false" max="50" min="50" style="0" width="10.8117647058824"/>
+    <col collapsed="false" hidden="false" max="51" min="51" style="0" width="8.10196078431373"/>
     <col collapsed="false" hidden="false" max="52" min="52" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="53" min="53" style="0" width="11.6274509803922"/>
+    <col collapsed="false" hidden="false" max="53" min="53" style="0" width="11.6666666666667"/>
     <col collapsed="false" hidden="false" max="54" min="54" style="0" width="5.52549019607843"/>
     <col collapsed="false" hidden="false" max="55" min="55" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="56" min="56" style="0" width="15.156862745098"/>
-    <col collapsed="false" hidden="false" max="57" min="57" style="0" width="10.7725490196078"/>
-    <col collapsed="false" hidden="false" max="58" min="58" style="0" width="8.09803921568627"/>
+    <col collapsed="false" hidden="false" max="56" min="56" style="0" width="15.2156862745098"/>
+    <col collapsed="false" hidden="false" max="57" min="57" style="0" width="10.8117647058824"/>
+    <col collapsed="false" hidden="false" max="58" min="58" style="0" width="8.10196078431373"/>
     <col collapsed="false" hidden="false" max="59" min="59" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="60" min="60" style="0" width="11.6274509803922"/>
+    <col collapsed="false" hidden="false" max="60" min="60" style="0" width="11.6666666666667"/>
     <col collapsed="false" hidden="false" max="61" min="61" style="0" width="5.52549019607843"/>
     <col collapsed="false" hidden="false" max="62" min="62" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="63" min="63" style="0" width="10.2745098039216"/>
-    <col collapsed="false" hidden="false" max="64" min="64" style="0" width="8.09803921568627"/>
+    <col collapsed="false" hidden="false" max="63" min="63" style="0" width="10.3137254901961"/>
+    <col collapsed="false" hidden="false" max="64" min="64" style="0" width="8.10196078431373"/>
     <col collapsed="false" hidden="false" max="65" min="65" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="66" min="66" style="0" width="11.6274509803922"/>
+    <col collapsed="false" hidden="false" max="66" min="66" style="0" width="11.6666666666667"/>
     <col collapsed="false" hidden="false" max="67" min="67" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="68" min="68" style="0" width="13.9764705882353"/>
-    <col collapsed="false" hidden="false" max="69" min="69" style="0" width="8.09803921568627"/>
+    <col collapsed="false" hidden="false" max="68" min="68" style="0" width="14.0274509803922"/>
+    <col collapsed="false" hidden="false" max="69" min="69" style="0" width="8.10196078431373"/>
     <col collapsed="false" hidden="false" max="70" min="70" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="71" min="71" style="0" width="11.6274509803922"/>
+    <col collapsed="false" hidden="false" max="71" min="71" style="0" width="11.6666666666667"/>
     <col collapsed="false" hidden="false" max="72" min="72" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="73" min="73" style="0" width="12.9607843137255"/>
-    <col collapsed="false" hidden="false" max="74" min="74" style="0" width="8.09803921568627"/>
+    <col collapsed="false" hidden="false" max="73" min="73" style="0" width="13.0117647058824"/>
+    <col collapsed="false" hidden="false" max="74" min="74" style="0" width="8.10196078431373"/>
     <col collapsed="false" hidden="false" max="75" min="75" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="76" min="76" style="0" width="11.6274509803922"/>
+    <col collapsed="false" hidden="false" max="76" min="76" style="0" width="11.6666666666667"/>
     <col collapsed="false" hidden="false" max="77" min="77" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="78" min="78" style="0" width="12.7960784313726"/>
-    <col collapsed="false" hidden="false" max="79" min="79" style="0" width="8.09803921568627"/>
+    <col collapsed="false" hidden="false" max="78" min="78" style="0" width="12.8352941176471"/>
+    <col collapsed="false" hidden="false" max="79" min="79" style="0" width="8.10196078431373"/>
     <col collapsed="false" hidden="false" max="80" min="80" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="81" min="81" style="0" width="11.6274509803922"/>
+    <col collapsed="false" hidden="false" max="81" min="81" style="0" width="11.6666666666667"/>
     <col collapsed="false" hidden="false" max="82" min="82" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="83" min="83" style="0" width="13.6549019607843"/>
-    <col collapsed="false" hidden="false" max="84" min="84" style="0" width="8.09803921568627"/>
+    <col collapsed="false" hidden="false" max="83" min="83" style="0" width="13.7058823529412"/>
+    <col collapsed="false" hidden="false" max="84" min="84" style="0" width="8.10196078431373"/>
     <col collapsed="false" hidden="false" max="85" min="85" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="86" min="86" style="0" width="11.6274509803922"/>
+    <col collapsed="false" hidden="false" max="86" min="86" style="0" width="11.6666666666667"/>
     <col collapsed="false" hidden="false" max="87" min="87" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="88" min="88" style="0" width="14.8156862745098"/>
-    <col collapsed="false" hidden="false" max="89" min="89" style="0" width="8.09803921568627"/>
+    <col collapsed="false" hidden="false" max="88" min="88" style="0" width="14.8745098039216"/>
+    <col collapsed="false" hidden="false" max="89" min="89" style="0" width="8.10196078431373"/>
     <col collapsed="false" hidden="false" max="90" min="90" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="91" min="91" style="0" width="11.6274509803922"/>
+    <col collapsed="false" hidden="false" max="91" min="91" style="0" width="11.6666666666667"/>
     <col collapsed="false" hidden="false" max="92" min="92" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="93" min="93" style="0" width="10.2745098039216"/>
-    <col collapsed="false" hidden="false" max="94" min="94" style="0" width="13.8039215686275"/>
-    <col collapsed="false" hidden="false" max="95" min="95" style="0" width="14.8156862745098"/>
-    <col collapsed="false" hidden="false" max="96" min="96" style="0" width="17.3490196078431"/>
+    <col collapsed="false" hidden="false" max="93" min="93" style="0" width="10.3137254901961"/>
+    <col collapsed="false" hidden="false" max="94" min="94" style="0" width="13.8509803921569"/>
+    <col collapsed="false" hidden="false" max="95" min="95" style="0" width="14.8745098039216"/>
+    <col collapsed="false" hidden="false" max="96" min="96" style="0" width="17.4274509803922"/>
     <col collapsed="false" hidden="false" max="97" min="97" style="0" width="6.02352941176471"/>
-    <col collapsed="false" hidden="false" max="98" min="98" style="0" width="23.0588235294118"/>
-    <col collapsed="false" hidden="false" max="99" min="99" style="0" width="16.0039215686275"/>
-    <col collapsed="false" hidden="false" max="100" min="100" style="0" width="17.1764705882353"/>
-    <col collapsed="false" hidden="false" max="101" min="101" style="0" width="17.3490196078431"/>
+    <col collapsed="false" hidden="false" max="98" min="98" style="0" width="23.156862745098"/>
+    <col collapsed="false" hidden="false" max="99" min="99" style="0" width="16.0705882352941"/>
+    <col collapsed="false" hidden="false" max="100" min="100" style="0" width="17.2509803921569"/>
+    <col collapsed="false" hidden="false" max="101" min="101" style="0" width="17.4274509803922"/>
     <col collapsed="false" hidden="false" max="102" min="102" style="0" width="6.02352941176471"/>
-    <col collapsed="false" hidden="false" max="103" min="103" style="0" width="22.2235294117647"/>
-    <col collapsed="false" hidden="false" max="104" min="104" style="0" width="16.0039215686275"/>
-    <col collapsed="false" hidden="false" max="105" min="105" style="0" width="17.1764705882353"/>
-    <col collapsed="false" hidden="false" max="106" min="106" style="0" width="17.3490196078431"/>
+    <col collapsed="false" hidden="false" max="103" min="103" style="0" width="22.3098039215686"/>
+    <col collapsed="false" hidden="false" max="104" min="104" style="0" width="16.0705882352941"/>
+    <col collapsed="false" hidden="false" max="105" min="105" style="0" width="17.2509803921569"/>
+    <col collapsed="false" hidden="false" max="106" min="106" style="0" width="17.4274509803922"/>
     <col collapsed="false" hidden="false" max="107" min="107" style="0" width="6.02352941176471"/>
-    <col collapsed="false" hidden="false" max="108" min="108" style="0" width="11.7843137254902"/>
-    <col collapsed="false" hidden="false" max="109" min="109" style="0" width="17.3490196078431"/>
-    <col collapsed="false" hidden="false" max="110" min="110" style="0" width="12.7960784313726"/>
-    <col collapsed="false" hidden="false" max="111" min="111" style="0" width="18.5294117647059"/>
-    <col collapsed="false" hidden="false" max="112" min="112" style="0" width="17.3490196078431"/>
-    <col collapsed="false" hidden="false" max="113" min="113" style="0" width="12.7960784313726"/>
-    <col collapsed="false" hidden="false" max="114" min="114" style="0" width="19.5411764705882"/>
-    <col collapsed="false" hidden="false" max="115" min="115" style="0" width="17.3490196078431"/>
-    <col collapsed="false" hidden="false" max="116" min="116" style="0" width="12.7960784313726"/>
-    <col collapsed="false" hidden="false" max="117" min="117" style="0" width="18.7058823529412"/>
-    <col collapsed="false" hidden="false" max="119" min="118" style="0" width="17.3490196078431"/>
-    <col collapsed="false" hidden="false" max="120" min="120" style="0" width="16.5019607843137"/>
-    <col collapsed="false" hidden="false" max="121" min="121" style="0" width="11.7843137254902"/>
-    <col collapsed="false" hidden="false" max="122" min="122" style="0" width="15.6705882352941"/>
-    <col collapsed="false" hidden="false" max="123" min="123" style="0" width="16.3372549019608"/>
-    <col collapsed="false" hidden="false" max="124" min="124" style="0" width="18.5294117647059"/>
-    <col collapsed="false" hidden="false" max="125" min="125" style="0" width="14.4745098039216"/>
-    <col collapsed="false" hidden="false" max="126" min="126" style="0" width="13.6549019607843"/>
-    <col collapsed="false" hidden="false" max="138" min="127" style="0" width="18.7058823529412"/>
-    <col collapsed="false" hidden="false" max="140" min="139" style="0" width="30.9960784313725"/>
-    <col collapsed="false" hidden="false" max="141" min="141" style="0" width="26.1137254901961"/>
-    <col collapsed="false" hidden="false" max="142" min="142" style="0" width="20.721568627451"/>
-    <col collapsed="false" hidden="false" max="143" min="143" style="0" width="13.1294117647059"/>
+    <col collapsed="false" hidden="false" max="108" min="108" style="0" width="11.8235294117647"/>
+    <col collapsed="false" hidden="false" max="109" min="109" style="0" width="17.4274509803922"/>
+    <col collapsed="false" hidden="false" max="110" min="110" style="0" width="12.8352941176471"/>
+    <col collapsed="false" hidden="false" max="111" min="111" style="0" width="18.6078431372549"/>
+    <col collapsed="false" hidden="false" max="112" min="112" style="0" width="17.4274509803922"/>
+    <col collapsed="false" hidden="false" max="113" min="113" style="0" width="12.8352941176471"/>
+    <col collapsed="false" hidden="false" max="114" min="114" style="0" width="19.6274509803922"/>
+    <col collapsed="false" hidden="false" max="115" min="115" style="0" width="17.4274509803922"/>
+    <col collapsed="false" hidden="false" max="116" min="116" style="0" width="12.8352941176471"/>
+    <col collapsed="false" hidden="false" max="117" min="117" style="0" width="18.7803921568627"/>
+    <col collapsed="false" hidden="false" max="119" min="118" style="0" width="17.4274509803922"/>
+    <col collapsed="false" hidden="false" max="120" min="120" style="0" width="16.5686274509804"/>
+    <col collapsed="false" hidden="false" max="121" min="121" style="0" width="11.8235294117647"/>
+    <col collapsed="false" hidden="false" max="122" min="122" style="0" width="15.7411764705882"/>
+    <col collapsed="false" hidden="false" max="123" min="123" style="0" width="16.4039215686274"/>
+    <col collapsed="false" hidden="false" max="124" min="124" style="0" width="18.6078431372549"/>
+    <col collapsed="false" hidden="false" max="125" min="125" style="0" width="14.5254901960784"/>
+    <col collapsed="false" hidden="false" max="126" min="126" style="0" width="13.7058823529412"/>
+    <col collapsed="false" hidden="false" max="138" min="127" style="0" width="18.7803921568627"/>
+    <col collapsed="false" hidden="false" max="140" min="139" style="0" width="31.1137254901961"/>
+    <col collapsed="false" hidden="false" max="141" min="141" style="0" width="26.2274509803922"/>
+    <col collapsed="false" hidden="false" max="142" min="142" style="0" width="20.8"/>
+    <col collapsed="false" hidden="false" max="143" min="143" style="0" width="13.1764705882353"/>
     <col collapsed="false" hidden="false" max="144" min="144" style="0" width="7.74117647058824"/>
-    <col collapsed="false" hidden="false" max="145" min="145" style="0" width="13.4627450980392"/>
-    <col collapsed="false" hidden="false" max="146" min="146" style="0" width="10.4392156862745"/>
-    <col collapsed="false" hidden="false" max="1025" min="147" style="0" width="18.7058823529412"/>
+    <col collapsed="false" hidden="false" max="145" min="145" style="0" width="13.5176470588235"/>
+    <col collapsed="false" hidden="false" max="146" min="146" style="0" width="10.478431372549"/>
+    <col collapsed="false" hidden="false" max="1025" min="147" style="0" width="18.7803921568627"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="1">
@@ -8549,13 +8549,13 @@
       </c>
       <c r="BK4" s="66"/>
       <c r="BL4" s="66" t="n">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="BM4" s="66" t="n">
         <v>200</v>
       </c>
       <c r="BN4" s="66" t="n">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="BO4" s="64"/>
       <c r="BP4" s="66"/>
@@ -8615,17 +8615,17 @@
       <c r="DN4" s="66"/>
       <c r="DO4" s="66"/>
       <c r="DP4" s="66" t="n">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="DQ4" s="66"/>
       <c r="DR4" s="66"/>
       <c r="DS4" s="66"/>
       <c r="DT4" s="66" t="n">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="DU4" s="66"/>
       <c r="DV4" s="66" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="DW4" s="66"/>
       <c r="DX4" s="66"/>
@@ -12384,145 +12384,145 @@
   </sheetPr>
   <dimension ref="A1:EP32"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="BB1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100">
+      <selection activeCell="BM7" activeCellId="0" pane="topLeft" sqref="BM7"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.1176470588235"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.2745098039216"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.93333333333333"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.0313725490196"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.9490196078431"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.4901960784314"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.4196078431373"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.4588235294118"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.6705882352941"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="18.7058823529412"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="15.3333333333333"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.6235294117647"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="11.956862745098"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="13.8039215686275"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="12.9607843137255"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.9764705882353"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="16.5019607843137"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.2901960784314"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="16.3372549019608"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="13.9764705882353"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="10.2745098039216"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="10.7725490196078"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="8.09803921568627"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.2313725490196"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.3137254901961"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.98039215686275"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.1098039215686"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.0666666666667"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.5372549019608"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.5176470588235"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.5058823529412"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.7411764705882"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="18.7803921568627"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="15.4"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.6627450980392"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="12"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="13.8509803921569"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="13.0117647058824"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="14.0274509803922"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="16.5686274509804"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.3294117647059"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="16.4039215686274"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="14.0274509803922"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="10.3137254901961"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="10.8117647058824"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="8.10196078431373"/>
     <col collapsed="false" hidden="false" max="24" min="24" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="11.6274509803922"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="11.6666666666667"/>
     <col collapsed="false" hidden="false" max="26" min="26" style="0" width="5.52549019607843"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="11.6274509803922"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="14.1411764705882"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="10.7725490196078"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="8.09803921568627"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="11.6666666666667"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="14.1921568627451"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="10.8117647058824"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="8.10196078431373"/>
     <col collapsed="false" hidden="false" max="31" min="31" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="11.6274509803922"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="11.6666666666667"/>
     <col collapsed="false" hidden="false" max="33" min="33" style="0" width="5.52549019607843"/>
     <col collapsed="false" hidden="false" max="34" min="34" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="14.6588235294118"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="10.7725490196078"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="8.09803921568627"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="14.7176470588235"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="10.8117647058824"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="8.10196078431373"/>
     <col collapsed="false" hidden="false" max="38" min="38" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="11.6274509803922"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="11.6666666666667"/>
     <col collapsed="false" hidden="false" max="40" min="40" style="0" width="5.52549019607843"/>
     <col collapsed="false" hidden="false" max="41" min="41" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="14.3176470588235"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="10.7725490196078"/>
-    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="8.09803921568627"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="14.3764705882353"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="10.8117647058824"/>
+    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="8.10196078431373"/>
     <col collapsed="false" hidden="false" max="45" min="45" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="11.6274509803922"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="11.6666666666667"/>
     <col collapsed="false" hidden="false" max="47" min="47" style="0" width="5.52549019607843"/>
     <col collapsed="false" hidden="false" max="48" min="48" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="49" min="49" style="0" width="14.8156862745098"/>
-    <col collapsed="false" hidden="false" max="50" min="50" style="0" width="10.7725490196078"/>
-    <col collapsed="false" hidden="false" max="51" min="51" style="0" width="8.09803921568627"/>
+    <col collapsed="false" hidden="false" max="49" min="49" style="0" width="14.8745098039216"/>
+    <col collapsed="false" hidden="false" max="50" min="50" style="0" width="10.8117647058824"/>
+    <col collapsed="false" hidden="false" max="51" min="51" style="0" width="8.10196078431373"/>
     <col collapsed="false" hidden="false" max="52" min="52" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="53" min="53" style="0" width="11.6274509803922"/>
+    <col collapsed="false" hidden="false" max="53" min="53" style="0" width="11.6666666666667"/>
     <col collapsed="false" hidden="false" max="54" min="54" style="0" width="5.52549019607843"/>
     <col collapsed="false" hidden="false" max="55" min="55" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="56" min="56" style="0" width="15.156862745098"/>
-    <col collapsed="false" hidden="false" max="57" min="57" style="0" width="10.7725490196078"/>
-    <col collapsed="false" hidden="false" max="58" min="58" style="0" width="8.09803921568627"/>
+    <col collapsed="false" hidden="false" max="56" min="56" style="0" width="15.2156862745098"/>
+    <col collapsed="false" hidden="false" max="57" min="57" style="0" width="10.8117647058824"/>
+    <col collapsed="false" hidden="false" max="58" min="58" style="0" width="8.10196078431373"/>
     <col collapsed="false" hidden="false" max="59" min="59" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="60" min="60" style="0" width="11.6274509803922"/>
+    <col collapsed="false" hidden="false" max="60" min="60" style="0" width="11.6666666666667"/>
     <col collapsed="false" hidden="false" max="61" min="61" style="0" width="5.52549019607843"/>
     <col collapsed="false" hidden="false" max="62" min="62" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="63" min="63" style="0" width="10.2745098039216"/>
-    <col collapsed="false" hidden="false" max="64" min="64" style="0" width="8.09803921568627"/>
+    <col collapsed="false" hidden="false" max="63" min="63" style="0" width="10.3137254901961"/>
+    <col collapsed="false" hidden="false" max="64" min="64" style="0" width="8.10196078431373"/>
     <col collapsed="false" hidden="false" max="65" min="65" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="66" min="66" style="0" width="11.6274509803922"/>
+    <col collapsed="false" hidden="false" max="66" min="66" style="0" width="11.6666666666667"/>
     <col collapsed="false" hidden="false" max="67" min="67" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="68" min="68" style="0" width="13.9764705882353"/>
-    <col collapsed="false" hidden="false" max="69" min="69" style="0" width="8.09803921568627"/>
+    <col collapsed="false" hidden="false" max="68" min="68" style="0" width="14.0274509803922"/>
+    <col collapsed="false" hidden="false" max="69" min="69" style="0" width="8.10196078431373"/>
     <col collapsed="false" hidden="false" max="70" min="70" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="71" min="71" style="0" width="11.6274509803922"/>
+    <col collapsed="false" hidden="false" max="71" min="71" style="0" width="11.6666666666667"/>
     <col collapsed="false" hidden="false" max="72" min="72" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="73" min="73" style="0" width="12.9607843137255"/>
-    <col collapsed="false" hidden="false" max="74" min="74" style="0" width="8.09803921568627"/>
+    <col collapsed="false" hidden="false" max="73" min="73" style="0" width="13.0117647058824"/>
+    <col collapsed="false" hidden="false" max="74" min="74" style="0" width="8.10196078431373"/>
     <col collapsed="false" hidden="false" max="75" min="75" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="76" min="76" style="0" width="11.6274509803922"/>
+    <col collapsed="false" hidden="false" max="76" min="76" style="0" width="11.6666666666667"/>
     <col collapsed="false" hidden="false" max="77" min="77" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="78" min="78" style="0" width="12.7960784313726"/>
-    <col collapsed="false" hidden="false" max="79" min="79" style="0" width="8.09803921568627"/>
+    <col collapsed="false" hidden="false" max="78" min="78" style="0" width="12.8352941176471"/>
+    <col collapsed="false" hidden="false" max="79" min="79" style="0" width="8.10196078431373"/>
     <col collapsed="false" hidden="false" max="80" min="80" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="81" min="81" style="0" width="11.6274509803922"/>
+    <col collapsed="false" hidden="false" max="81" min="81" style="0" width="11.6666666666667"/>
     <col collapsed="false" hidden="false" max="82" min="82" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="83" min="83" style="0" width="13.6549019607843"/>
-    <col collapsed="false" hidden="false" max="84" min="84" style="0" width="8.09803921568627"/>
+    <col collapsed="false" hidden="false" max="83" min="83" style="0" width="13.7058823529412"/>
+    <col collapsed="false" hidden="false" max="84" min="84" style="0" width="8.10196078431373"/>
     <col collapsed="false" hidden="false" max="85" min="85" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="86" min="86" style="0" width="11.6274509803922"/>
+    <col collapsed="false" hidden="false" max="86" min="86" style="0" width="11.6666666666667"/>
     <col collapsed="false" hidden="false" max="87" min="87" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="88" min="88" style="0" width="14.8156862745098"/>
-    <col collapsed="false" hidden="false" max="89" min="89" style="0" width="8.09803921568627"/>
+    <col collapsed="false" hidden="false" max="88" min="88" style="0" width="14.8745098039216"/>
+    <col collapsed="false" hidden="false" max="89" min="89" style="0" width="8.10196078431373"/>
     <col collapsed="false" hidden="false" max="90" min="90" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="91" min="91" style="0" width="11.6274509803922"/>
+    <col collapsed="false" hidden="false" max="91" min="91" style="0" width="11.6666666666667"/>
     <col collapsed="false" hidden="false" max="92" min="92" style="0" width="5.2156862745098"/>
-    <col collapsed="false" hidden="false" max="93" min="93" style="0" width="10.2745098039216"/>
-    <col collapsed="false" hidden="false" max="94" min="94" style="0" width="13.8039215686275"/>
-    <col collapsed="false" hidden="false" max="95" min="95" style="0" width="14.8156862745098"/>
-    <col collapsed="false" hidden="false" max="96" min="96" style="0" width="17.3490196078431"/>
+    <col collapsed="false" hidden="false" max="93" min="93" style="0" width="10.3137254901961"/>
+    <col collapsed="false" hidden="false" max="94" min="94" style="0" width="13.8509803921569"/>
+    <col collapsed="false" hidden="false" max="95" min="95" style="0" width="14.8745098039216"/>
+    <col collapsed="false" hidden="false" max="96" min="96" style="0" width="17.4274509803922"/>
     <col collapsed="false" hidden="false" max="97" min="97" style="0" width="6.02352941176471"/>
-    <col collapsed="false" hidden="false" max="98" min="98" style="0" width="23.0588235294118"/>
-    <col collapsed="false" hidden="false" max="99" min="99" style="0" width="16.0039215686275"/>
-    <col collapsed="false" hidden="false" max="100" min="100" style="0" width="17.1764705882353"/>
-    <col collapsed="false" hidden="false" max="101" min="101" style="0" width="17.3490196078431"/>
+    <col collapsed="false" hidden="false" max="98" min="98" style="0" width="23.156862745098"/>
+    <col collapsed="false" hidden="false" max="99" min="99" style="0" width="16.0705882352941"/>
+    <col collapsed="false" hidden="false" max="100" min="100" style="0" width="17.2509803921569"/>
+    <col collapsed="false" hidden="false" max="101" min="101" style="0" width="17.4274509803922"/>
     <col collapsed="false" hidden="false" max="102" min="102" style="0" width="6.02352941176471"/>
-    <col collapsed="false" hidden="false" max="103" min="103" style="0" width="22.2235294117647"/>
-    <col collapsed="false" hidden="false" max="104" min="104" style="0" width="16.0039215686275"/>
-    <col collapsed="false" hidden="false" max="105" min="105" style="0" width="17.1764705882353"/>
-    <col collapsed="false" hidden="false" max="106" min="106" style="0" width="17.3490196078431"/>
+    <col collapsed="false" hidden="false" max="103" min="103" style="0" width="22.3098039215686"/>
+    <col collapsed="false" hidden="false" max="104" min="104" style="0" width="16.0705882352941"/>
+    <col collapsed="false" hidden="false" max="105" min="105" style="0" width="17.2509803921569"/>
+    <col collapsed="false" hidden="false" max="106" min="106" style="0" width="17.4274509803922"/>
     <col collapsed="false" hidden="false" max="107" min="107" style="0" width="6.02352941176471"/>
-    <col collapsed="false" hidden="false" max="108" min="108" style="0" width="11.7843137254902"/>
-    <col collapsed="false" hidden="false" max="109" min="109" style="0" width="17.3490196078431"/>
-    <col collapsed="false" hidden="false" max="110" min="110" style="0" width="12.7960784313726"/>
-    <col collapsed="false" hidden="false" max="111" min="111" style="0" width="18.5294117647059"/>
-    <col collapsed="false" hidden="false" max="112" min="112" style="0" width="17.3490196078431"/>
-    <col collapsed="false" hidden="false" max="113" min="113" style="0" width="12.7960784313726"/>
-    <col collapsed="false" hidden="false" max="114" min="114" style="0" width="19.5411764705882"/>
-    <col collapsed="false" hidden="false" max="115" min="115" style="0" width="17.3490196078431"/>
-    <col collapsed="false" hidden="false" max="116" min="116" style="0" width="12.7960784313726"/>
-    <col collapsed="false" hidden="false" max="117" min="117" style="0" width="18.7058823529412"/>
-    <col collapsed="false" hidden="false" max="119" min="118" style="0" width="17.3490196078431"/>
-    <col collapsed="false" hidden="false" max="120" min="120" style="0" width="16.5019607843137"/>
-    <col collapsed="false" hidden="false" max="121" min="121" style="0" width="11.7843137254902"/>
-    <col collapsed="false" hidden="false" max="122" min="122" style="0" width="15.6705882352941"/>
-    <col collapsed="false" hidden="false" max="123" min="123" style="0" width="16.3372549019608"/>
-    <col collapsed="false" hidden="false" max="124" min="124" style="0" width="18.5294117647059"/>
-    <col collapsed="false" hidden="false" max="125" min="125" style="0" width="14.4745098039216"/>
-    <col collapsed="false" hidden="false" max="126" min="126" style="0" width="13.6549019607843"/>
-    <col collapsed="false" hidden="false" max="138" min="127" style="0" width="18.7058823529412"/>
-    <col collapsed="false" hidden="false" max="140" min="139" style="0" width="30.9960784313725"/>
-    <col collapsed="false" hidden="false" max="141" min="141" style="0" width="26.1137254901961"/>
-    <col collapsed="false" hidden="false" max="142" min="142" style="0" width="20.721568627451"/>
-    <col collapsed="false" hidden="false" max="143" min="143" style="0" width="13.1294117647059"/>
+    <col collapsed="false" hidden="false" max="108" min="108" style="0" width="11.8235294117647"/>
+    <col collapsed="false" hidden="false" max="109" min="109" style="0" width="17.4274509803922"/>
+    <col collapsed="false" hidden="false" max="110" min="110" style="0" width="12.8352941176471"/>
+    <col collapsed="false" hidden="false" max="111" min="111" style="0" width="18.6078431372549"/>
+    <col collapsed="false" hidden="false" max="112" min="112" style="0" width="17.4274509803922"/>
+    <col collapsed="false" hidden="false" max="113" min="113" style="0" width="12.8352941176471"/>
+    <col collapsed="false" hidden="false" max="114" min="114" style="0" width="19.6274509803922"/>
+    <col collapsed="false" hidden="false" max="115" min="115" style="0" width="17.4274509803922"/>
+    <col collapsed="false" hidden="false" max="116" min="116" style="0" width="12.8352941176471"/>
+    <col collapsed="false" hidden="false" max="117" min="117" style="0" width="18.7803921568627"/>
+    <col collapsed="false" hidden="false" max="119" min="118" style="0" width="17.4274509803922"/>
+    <col collapsed="false" hidden="false" max="120" min="120" style="0" width="16.5686274509804"/>
+    <col collapsed="false" hidden="false" max="121" min="121" style="0" width="11.8235294117647"/>
+    <col collapsed="false" hidden="false" max="122" min="122" style="0" width="15.7411764705882"/>
+    <col collapsed="false" hidden="false" max="123" min="123" style="0" width="16.4039215686274"/>
+    <col collapsed="false" hidden="false" max="124" min="124" style="0" width="18.6078431372549"/>
+    <col collapsed="false" hidden="false" max="125" min="125" style="0" width="14.5254901960784"/>
+    <col collapsed="false" hidden="false" max="126" min="126" style="0" width="13.7058823529412"/>
+    <col collapsed="false" hidden="false" max="138" min="127" style="0" width="18.7803921568627"/>
+    <col collapsed="false" hidden="false" max="140" min="139" style="0" width="31.1137254901961"/>
+    <col collapsed="false" hidden="false" max="141" min="141" style="0" width="26.2274509803922"/>
+    <col collapsed="false" hidden="false" max="142" min="142" style="0" width="20.8"/>
+    <col collapsed="false" hidden="false" max="143" min="143" style="0" width="13.1764705882353"/>
     <col collapsed="false" hidden="false" max="144" min="144" style="0" width="7.74117647058824"/>
-    <col collapsed="false" hidden="false" max="145" min="145" style="0" width="13.4627450980392"/>
-    <col collapsed="false" hidden="false" max="146" min="146" style="0" width="10.4392156862745"/>
-    <col collapsed="false" hidden="false" max="1025" min="147" style="0" width="18.7058823529412"/>
+    <col collapsed="false" hidden="false" max="145" min="145" style="0" width="13.5176470588235"/>
+    <col collapsed="false" hidden="false" max="146" min="146" style="0" width="10.478431372549"/>
+    <col collapsed="false" hidden="false" max="1025" min="147" style="0" width="18.7803921568627"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="1">
@@ -13364,7 +13364,7 @@
         <v>2</v>
       </c>
       <c r="Y4" s="66" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Z4" s="65" t="s">
         <v>54</v>
@@ -13422,7 +13422,7 @@
         <v>100</v>
       </c>
       <c r="BM4" s="66" t="n">
-        <v>200</v>
+        <v>3</v>
       </c>
       <c r="BN4" s="66" t="n">
         <v>300</v>

</xml_diff>